<commit_message>
feat: added data-driven for flow 7
</commit_message>
<xml_diff>
--- a/src/test/resources/CourseraAutomationData.xlsx
+++ b/src/test/resources/CourseraAutomationData.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Personal\Automation\workspace\CourseraAutomation\src\test\resources\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{56A440DF-6C2E-48B5-AADB-50C47135D853}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5EAA36FC-AFB9-49E5-AD2E-72E1CEBB54F1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" firstSheet="3" activeTab="6" xr2:uid="{8CA69206-0C49-4EFD-98F1-4AF42D798B8E}"/>
   </bookViews>
@@ -43,7 +43,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="100" uniqueCount="89">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="99" uniqueCount="89">
   <si>
     <t>Language</t>
   </si>
@@ -1104,11 +1104,14 @@
   <dimension ref="A1:G9"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H7" sqref="H7"/>
+      <selection activeCell="H11" sqref="H11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
+    <col min="1" max="1" customWidth="true" width="25.26953125"/>
+    <col min="2" max="2" customWidth="true" width="15.54296875"/>
+    <col min="3" max="3" customWidth="true" width="13.26953125"/>
     <col min="4" max="4" customWidth="true" width="23.36328125"/>
     <col min="5" max="5" customWidth="true" width="13.6328125"/>
     <col min="6" max="6" customWidth="true" width="16.0"/>

</xml_diff>

<commit_message>
feat: excel data-driven for flow 7 and 9
</commit_message>
<xml_diff>
--- a/src/test/resources/CourseraAutomationData.xlsx
+++ b/src/test/resources/CourseraAutomationData.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Personal\Automation\workspace\CourseraAutomation\src\test\resources\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5EAA36FC-AFB9-49E5-AD2E-72E1CEBB54F1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DA404112-ABAD-4DA1-A910-93B6F80027F0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" firstSheet="3" activeTab="6" xr2:uid="{8CA69206-0C49-4EFD-98F1-4AF42D798B8E}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" firstSheet="4" activeTab="7" xr2:uid="{8CA69206-0C49-4EFD-98F1-4AF42D798B8E}"/>
   </bookViews>
   <sheets>
     <sheet name="CourseDetails" sheetId="1" r:id="rId1"/>
@@ -20,7 +20,7 @@
     <sheet name="OnlineDegree" sheetId="5" r:id="rId5"/>
     <sheet name="BusinessPlan" sheetId="6" r:id="rId6"/>
     <sheet name="CourseDetailedInfo" sheetId="7" r:id="rId7"/>
-    <sheet name="Sheet8" sheetId="8" r:id="rId8"/>
+    <sheet name="FooterValidation" sheetId="8" r:id="rId8"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -43,7 +43,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="99" uniqueCount="89">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="257" uniqueCount="245">
   <si>
     <t>Language</t>
   </si>
@@ -310,6 +310,474 @@
   </si>
   <si>
     <t>Develop dynamic and interactive web pages using JavaScript, including DOM manipulation, form validation, and client-side scripting techniques.</t>
+  </si>
+  <si>
+    <t>Link</t>
+  </si>
+  <si>
+    <t>Section</t>
+  </si>
+  <si>
+    <t>More</t>
+  </si>
+  <si>
+    <t>Privacy</t>
+  </si>
+  <si>
+    <t>https://www.coursera.org/about/privacy</t>
+  </si>
+  <si>
+    <t>Manage Cookie Preferences</t>
+  </si>
+  <si>
+    <t>https://www.coursera.org/about/cookies-manage</t>
+  </si>
+  <si>
+    <t>Investors</t>
+  </si>
+  <si>
+    <t>https://investor.coursera.com/</t>
+  </si>
+  <si>
+    <t>Help</t>
+  </si>
+  <si>
+    <t>https://learner.coursera.help/hc</t>
+  </si>
+  <si>
+    <t>Accessibility</t>
+  </si>
+  <si>
+    <t>https://learner.coursera.help/hc/articles/360050668591-Accessibility-Statement</t>
+  </si>
+  <si>
+    <t>Articles</t>
+  </si>
+  <si>
+    <t>https://www.coursera.org/articles</t>
+  </si>
+  <si>
+    <t>Modern Slavery Statement</t>
+  </si>
+  <si>
+    <t>https://coursera_assets.s3.amazonaws.com/footer/Modern+Slavery+Statement+(approved+March+26%2C+2025).pdf</t>
+  </si>
+  <si>
+    <t>Affiliates</t>
+  </si>
+  <si>
+    <t>https://about.coursera.org/affiliates</t>
+  </si>
+  <si>
+    <t>Terms</t>
+  </si>
+  <si>
+    <t>https://www.coursera.org/about/terms</t>
+  </si>
+  <si>
+    <t>Press</t>
+  </si>
+  <si>
+    <t>https://www.coursera.org/about/press</t>
+  </si>
+  <si>
+    <t>Contact</t>
+  </si>
+  <si>
+    <t>https://www.coursera.org/about/contact</t>
+  </si>
+  <si>
+    <t>Directory</t>
+  </si>
+  <si>
+    <t>https://www.coursera.org/directory</t>
+  </si>
+  <si>
+    <t>Career Resources</t>
+  </si>
+  <si>
+    <t>How to Learn Artificial Intelligence</t>
+  </si>
+  <si>
+    <t>https://www.coursera.org/articles/how-to-learn-artificial-intelligence</t>
+  </si>
+  <si>
+    <t>Share your Coursera Learning Story</t>
+  </si>
+  <si>
+    <t>https://airtable.com/appxSsG2Dz9CjSpF8/pagCDDP2Uinw59CNP/form</t>
+  </si>
+  <si>
+    <t>Popular Cybersecurity Certifications</t>
+  </si>
+  <si>
+    <t>https://www.coursera.org/articles/popular-cybersecurity-certifications</t>
+  </si>
+  <si>
+    <t>How to Get a PMP Certification</t>
+  </si>
+  <si>
+    <t>https://www.coursera.org/articles/the-pmp-certification-a-guide-to-getting-started</t>
+  </si>
+  <si>
+    <t>Career Aptitude Test</t>
+  </si>
+  <si>
+    <t>https://www.coursera.org/resources/career-quiz</t>
+  </si>
+  <si>
+    <t>Career Development Resources</t>
+  </si>
+  <si>
+    <t>https://www.coursera.org/resources</t>
+  </si>
+  <si>
+    <t>Popular Data Analytics Certifications</t>
+  </si>
+  <si>
+    <t>https://www.coursera.org/articles/data-analytics-certification</t>
+  </si>
+  <si>
+    <t>Essential IT Certifications</t>
+  </si>
+  <si>
+    <t>https://www.coursera.org/articles/essential-it-certifications-entry-level-and-beginner</t>
+  </si>
+  <si>
+    <t>What Does a Data Analyst Do?</t>
+  </si>
+  <si>
+    <t>https://www.coursera.org/articles/what-does-a-data-analyst-do-a-career-guide</t>
+  </si>
+  <si>
+    <t>High-Income Skills to Learn</t>
+  </si>
+  <si>
+    <t>https://www.coursera.org/articles/high-income-skills</t>
+  </si>
+  <si>
+    <t>Analytical Skills</t>
+  </si>
+  <si>
+    <t>Data Science</t>
+  </si>
+  <si>
+    <t>https://www.coursera.org/courses?query=data%20science&amp;topic=Data%20Science</t>
+  </si>
+  <si>
+    <t>Artificial Intelligence</t>
+  </si>
+  <si>
+    <t>https://www.coursera.org/courses?query=artificial%20intelligence</t>
+  </si>
+  <si>
+    <t>Microsoft Power BI</t>
+  </si>
+  <si>
+    <t>https://www.coursera.org/courses?query=microsoft%20power%20bi</t>
+  </si>
+  <si>
+    <t>Big Data</t>
+  </si>
+  <si>
+    <t>https://www.coursera.org/courses?query=big%20data</t>
+  </si>
+  <si>
+    <t>Financial Modeling</t>
+  </si>
+  <si>
+    <t>https://www.coursera.org/courses?query=financial%20modeling</t>
+  </si>
+  <si>
+    <t>Data Analytics</t>
+  </si>
+  <si>
+    <t>https://www.coursera.org/courses?query=data%20analytics</t>
+  </si>
+  <si>
+    <t>Machine Learning</t>
+  </si>
+  <si>
+    <t>https://www.coursera.org/courses?query=machine%20learning&amp;skills=Machine%20Learning</t>
+  </si>
+  <si>
+    <t>Microsoft Excel</t>
+  </si>
+  <si>
+    <t>https://www.coursera.org/courses?query=microsoft%20excel</t>
+  </si>
+  <si>
+    <t>Business Analysis</t>
+  </si>
+  <si>
+    <t>https://www.coursera.org/courses?query=business%20analysis</t>
+  </si>
+  <si>
+    <t>SQL</t>
+  </si>
+  <si>
+    <t>https://www.coursera.org/courses?query=sql</t>
+  </si>
+  <si>
+    <t>Technical Skills</t>
+  </si>
+  <si>
+    <t>Ethical Hacking</t>
+  </si>
+  <si>
+    <t>https://www.coursera.org/courses?query=ethical%20hacking</t>
+  </si>
+  <si>
+    <t>DevOps</t>
+  </si>
+  <si>
+    <t>https://www.coursera.org/courses?query=devops</t>
+  </si>
+  <si>
+    <t>Generative AI</t>
+  </si>
+  <si>
+    <t>https://www.coursera.org/courses?query=generative%20ai</t>
+  </si>
+  <si>
+    <t>ChatGPT</t>
+  </si>
+  <si>
+    <t>https://www.coursera.org/courses?query=chatgpt</t>
+  </si>
+  <si>
+    <t>Coding</t>
+  </si>
+  <si>
+    <t>https://www.coursera.org/courses?query=coding</t>
+  </si>
+  <si>
+    <t>Computer Science</t>
+  </si>
+  <si>
+    <t>https://www.coursera.org/courses?query=computer%20science&amp;topic=Computer%20Science</t>
+  </si>
+  <si>
+    <t>Java Programming</t>
+  </si>
+  <si>
+    <t>https://www.coursera.org/courses?query=java</t>
+  </si>
+  <si>
+    <t>Cybersecurity</t>
+  </si>
+  <si>
+    <t>https://www.coursera.org/courses?query=cybersecurity</t>
+  </si>
+  <si>
+    <t>https://www.coursera.org/courses?query=web%20development</t>
+  </si>
+  <si>
+    <t>Python</t>
+  </si>
+  <si>
+    <t>https://www.coursera.org/courses?query=python</t>
+  </si>
+  <si>
+    <t>Business Skills</t>
+  </si>
+  <si>
+    <t>Google</t>
+  </si>
+  <si>
+    <t>https://www.coursera.org/courses?query=google</t>
+  </si>
+  <si>
+    <t>Project Management</t>
+  </si>
+  <si>
+    <t>https://www.coursera.org/courses?query=project%20management</t>
+  </si>
+  <si>
+    <t>Accounting</t>
+  </si>
+  <si>
+    <t>https://www.coursera.org/courses?query=accounting</t>
+  </si>
+  <si>
+    <t>IBM</t>
+  </si>
+  <si>
+    <t>https://www.coursera.org/courses?query=ibm</t>
+  </si>
+  <si>
+    <t>Finance</t>
+  </si>
+  <si>
+    <t>https://www.coursera.org/courses?query=finance&amp;skills=Finance</t>
+  </si>
+  <si>
+    <t>E-commerce</t>
+  </si>
+  <si>
+    <t>https://www.coursera.org/courses?query=e-commerce</t>
+  </si>
+  <si>
+    <t>Digital Marketing</t>
+  </si>
+  <si>
+    <t>https://www.coursera.org/courses?query=digital%20marketing</t>
+  </si>
+  <si>
+    <t>Social Media Marketing</t>
+  </si>
+  <si>
+    <t>https://www.coursera.org/courses?query=social%20media%20marketing</t>
+  </si>
+  <si>
+    <t>Graphic Design</t>
+  </si>
+  <si>
+    <t>https://www.coursera.org/courses?query=graphic%20design</t>
+  </si>
+  <si>
+    <t>Marketing</t>
+  </si>
+  <si>
+    <t>https://www.coursera.org/courses?query=marketing&amp;skills=Marketing</t>
+  </si>
+  <si>
+    <t>Community</t>
+  </si>
+  <si>
+    <t>Partners</t>
+  </si>
+  <si>
+    <t>https://www.coursera.org/partners</t>
+  </si>
+  <si>
+    <t>Tech Blog</t>
+  </si>
+  <si>
+    <t>https://medium.com/coursera-engineering</t>
+  </si>
+  <si>
+    <t>The Coursera Podcast</t>
+  </si>
+  <si>
+    <t>https://open.spotify.com/show/58M36bneU7REOofdPZxe6A</t>
+  </si>
+  <si>
+    <t>Beta Testers</t>
+  </si>
+  <si>
+    <t>https://www.coursera.support/s/article/360000152926-Become-a-Coursera-beta-tester</t>
+  </si>
+  <si>
+    <t>Learners</t>
+  </si>
+  <si>
+    <t>https://www.coursera.community/</t>
+  </si>
+  <si>
+    <t>Blog</t>
+  </si>
+  <si>
+    <t>https://blog.coursera.org/</t>
+  </si>
+  <si>
+    <t>Coursera</t>
+  </si>
+  <si>
+    <t>MasterTrack® Certificates</t>
+  </si>
+  <si>
+    <t>https://www.coursera.org/mastertrack</t>
+  </si>
+  <si>
+    <t>Leadership</t>
+  </si>
+  <si>
+    <t>https://about.coursera.org/leadership</t>
+  </si>
+  <si>
+    <t>Coursera Plus</t>
+  </si>
+  <si>
+    <t>https://www.coursera.org/courseraplus</t>
+  </si>
+  <si>
+    <t>Degrees</t>
+  </si>
+  <si>
+    <t>https://www.coursera.org/degrees</t>
+  </si>
+  <si>
+    <t>Become a Partner</t>
+  </si>
+  <si>
+    <t>https://partnerships.coursera.org/?utm_medium=coursera&amp;utm_source=partnerships&amp;utm_campaign=website&amp;utm_content=corp-to-home-footer-become-a-partner</t>
+  </si>
+  <si>
+    <t>For Enterprise</t>
+  </si>
+  <si>
+    <t>https://www.coursera.org/business?utm_campaign=website&amp;utm_content=corp-to-home-footer-for-enterprise&amp;utm_medium=coursera&amp;utm_source=enterprise</t>
+  </si>
+  <si>
+    <t>Careers</t>
+  </si>
+  <si>
+    <t>https://careers.coursera.com/</t>
+  </si>
+  <si>
+    <t>Professional Certificates</t>
+  </si>
+  <si>
+    <t>https://www.coursera.org/professional-certificate</t>
+  </si>
+  <si>
+    <t>What We Offer</t>
+  </si>
+  <si>
+    <t>https://about.coursera.org/how-coursera-works/</t>
+  </si>
+  <si>
+    <t>Catalog</t>
+  </si>
+  <si>
+    <t>https://www.coursera.org/browse</t>
+  </si>
+  <si>
+    <t>About</t>
+  </si>
+  <si>
+    <t>https://about.coursera.org/</t>
+  </si>
+  <si>
+    <t>For Government</t>
+  </si>
+  <si>
+    <t>https://www.coursera.org/government?utm_campaign=website&amp;utm_content=corp-to-home-footer-for-government&amp;utm_medium=coursera&amp;utm_source=enterprise</t>
+  </si>
+  <si>
+    <t>Social Impact</t>
+  </si>
+  <si>
+    <t>https://www.coursera.org/social-impact</t>
+  </si>
+  <si>
+    <t>ECTS Credit Recommendations</t>
+  </si>
+  <si>
+    <t>https://www.coursera.org/explore/ects-credit-recommendation</t>
+  </si>
+  <si>
+    <t>For Campus</t>
+  </si>
+  <si>
+    <t>https://www.coursera.org/campus?utm_campaign=website&amp;utm_content=corp-to-home-footer-for-campus&amp;utm_medium=coursera&amp;utm_source=enterprise</t>
+  </si>
+  <si>
+    <t>Free Courses</t>
+  </si>
+  <si>
+    <t>https://www.coursera.org/courses?query=free</t>
   </si>
 </sst>
 </file>
@@ -317,7 +785,7 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="0"/>
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -332,8 +800,16 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color theme="10"/>
+      <name val="Aptos Narrow"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="5">
+  <fills count="7">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -358,6 +834,16 @@
         <bgColor rgb="FF000000"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="none">
+        <fgColor indexed="17"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor indexed="17"/>
+      </patternFill>
+    </fill>
   </fills>
   <borders count="1">
     <border>
@@ -368,17 +854,28 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="14">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="1" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFill="true"/>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="2">
+    <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -1103,7 +1600,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C731EF70-8147-435C-A429-F5FA1E52B0A3}">
   <dimension ref="A1:G9"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="H11" sqref="H11"/>
     </sheetView>
   </sheetViews>
@@ -1166,7 +1663,7 @@
         <v>85</v>
       </c>
     </row>
-    <row r="3">
+    <row r="3" spans="1:7" x14ac:dyDescent="0.35">
       <c r="F3" t="s" s="0">
         <v>79</v>
       </c>
@@ -1174,7 +1671,7 @@
         <v>86</v>
       </c>
     </row>
-    <row r="4">
+    <row r="4" spans="1:7" x14ac:dyDescent="0.35">
       <c r="F4" t="s" s="0">
         <v>80</v>
       </c>
@@ -1182,7 +1679,7 @@
         <v>87</v>
       </c>
     </row>
-    <row r="5">
+    <row r="5" spans="1:7" x14ac:dyDescent="0.35">
       <c r="F5" t="s" s="0">
         <v>81</v>
       </c>
@@ -1190,22 +1687,22 @@
         <v>88</v>
       </c>
     </row>
-    <row r="6">
+    <row r="6" spans="1:7" x14ac:dyDescent="0.35">
       <c r="F6" t="s" s="0">
         <v>82</v>
       </c>
     </row>
-    <row r="7">
+    <row r="7" spans="1:7" x14ac:dyDescent="0.35">
       <c r="F7" t="s" s="0">
         <v>83</v>
       </c>
     </row>
-    <row r="8">
+    <row r="8" spans="1:7" x14ac:dyDescent="0.35">
       <c r="F8" t="s" s="0">
         <v>84</v>
       </c>
     </row>
-    <row r="9">
+    <row r="9" spans="1:7" x14ac:dyDescent="0.35">
       <c r="F9" t="s" s="0">
         <v>7</v>
       </c>
@@ -1217,22 +1714,789 @@
 
 <file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{862E717F-3689-4B45-860F-E68FE6F4C7A7}">
-  <dimension ref="A1"/>
+  <dimension ref="A1:D75"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection sqref="A1:G2"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B13" sqref="B13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
     <col min="1" max="1" bestFit="true" customWidth="true" width="15.6328125"/>
+    <col min="2" max="2" customWidth="true" width="41.7265625"/>
     <col min="3" max="3" customWidth="true" width="10.26953125"/>
     <col min="4" max="4" customWidth="true" width="16.6328125"/>
     <col min="5" max="5" customWidth="true" width="19.26953125"/>
     <col min="6" max="6" customWidth="true" width="20.6328125"/>
     <col min="7" max="7" customWidth="true" width="14.81640625"/>
   </cols>
-  <sheetData/>
+  <sheetData>
+    <row r="1" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A1" t="s" s="0">
+        <v>90</v>
+      </c>
+      <c r="B1" s="4" t="s">
+        <v>4</v>
+      </c>
+      <c r="C1" s="4" t="s">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A2" s="7" t="s">
+        <v>91</v>
+      </c>
+      <c r="B2" s="6" t="s">
+        <v>92</v>
+      </c>
+      <c r="C2" s="6" t="s">
+        <v>93</v>
+      </c>
+      <c r="D2" s="6"/>
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A3" s="6"/>
+      <c r="B3" s="6" t="s">
+        <v>94</v>
+      </c>
+      <c r="C3" s="6" t="s">
+        <v>95</v>
+      </c>
+      <c r="D3" s="6"/>
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A4" s="6"/>
+      <c r="B4" s="6" t="s">
+        <v>96</v>
+      </c>
+      <c r="C4" s="6" t="s">
+        <v>97</v>
+      </c>
+      <c r="D4" s="6"/>
+    </row>
+    <row r="5" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A5" s="6"/>
+      <c r="B5" s="6" t="s">
+        <v>98</v>
+      </c>
+      <c r="C5" s="6" t="s">
+        <v>99</v>
+      </c>
+      <c r="D5" s="6"/>
+    </row>
+    <row r="6" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A6" s="6"/>
+      <c r="B6" s="6" t="s">
+        <v>100</v>
+      </c>
+      <c r="C6" s="6" t="s">
+        <v>101</v>
+      </c>
+      <c r="D6" s="6"/>
+    </row>
+    <row r="7" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A7" s="6"/>
+      <c r="B7" s="6" t="s">
+        <v>102</v>
+      </c>
+      <c r="C7" s="6" t="s">
+        <v>103</v>
+      </c>
+      <c r="D7" s="6"/>
+    </row>
+    <row r="8" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A8" s="6"/>
+      <c r="B8" s="6" t="s">
+        <v>104</v>
+      </c>
+      <c r="C8" s="6" t="s">
+        <v>105</v>
+      </c>
+      <c r="D8" s="6"/>
+    </row>
+    <row r="9" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A9" s="6"/>
+      <c r="B9" s="6" t="s">
+        <v>106</v>
+      </c>
+      <c r="C9" s="6" t="s">
+        <v>107</v>
+      </c>
+      <c r="D9" s="6"/>
+    </row>
+    <row r="10" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A10" s="6"/>
+      <c r="B10" s="6" t="s">
+        <v>108</v>
+      </c>
+      <c r="C10" s="6" t="s">
+        <v>109</v>
+      </c>
+      <c r="D10" s="6"/>
+    </row>
+    <row r="11" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A11" s="6"/>
+      <c r="B11" s="6" t="s">
+        <v>110</v>
+      </c>
+      <c r="C11" s="6" t="s">
+        <v>111</v>
+      </c>
+      <c r="D11" s="6"/>
+    </row>
+    <row r="12" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A12" s="6"/>
+      <c r="B12" s="6" t="s">
+        <v>112</v>
+      </c>
+      <c r="C12" s="6" t="s">
+        <v>113</v>
+      </c>
+      <c r="D12" s="6"/>
+    </row>
+    <row r="13" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A13" s="6"/>
+      <c r="B13" s="6" t="s">
+        <v>114</v>
+      </c>
+      <c r="C13" s="6" t="s">
+        <v>115</v>
+      </c>
+      <c r="D13" s="6"/>
+    </row>
+    <row r="14" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A14" s="8" t="s">
+        <v>116</v>
+      </c>
+      <c r="B14" s="6" t="s">
+        <v>117</v>
+      </c>
+      <c r="C14" s="6" t="s">
+        <v>118</v>
+      </c>
+      <c r="D14" s="6"/>
+    </row>
+    <row r="15" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A15" s="6"/>
+      <c r="B15" s="6" t="s">
+        <v>119</v>
+      </c>
+      <c r="C15" s="6" t="s">
+        <v>120</v>
+      </c>
+      <c r="D15" s="6"/>
+    </row>
+    <row r="16" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A16" s="6"/>
+      <c r="B16" s="6" t="s">
+        <v>121</v>
+      </c>
+      <c r="C16" s="6" t="s">
+        <v>122</v>
+      </c>
+      <c r="D16" s="6"/>
+    </row>
+    <row r="17" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A17" s="6"/>
+      <c r="B17" s="6" t="s">
+        <v>123</v>
+      </c>
+      <c r="C17" s="6" t="s">
+        <v>124</v>
+      </c>
+      <c r="D17" s="6"/>
+    </row>
+    <row r="18" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A18" s="6"/>
+      <c r="B18" s="6" t="s">
+        <v>125</v>
+      </c>
+      <c r="C18" s="6" t="s">
+        <v>126</v>
+      </c>
+      <c r="D18" s="6"/>
+    </row>
+    <row r="19" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A19" s="6"/>
+      <c r="B19" s="6" t="s">
+        <v>127</v>
+      </c>
+      <c r="C19" s="6" t="s">
+        <v>128</v>
+      </c>
+      <c r="D19" s="6"/>
+    </row>
+    <row r="20" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A20" s="6"/>
+      <c r="B20" s="6" t="s">
+        <v>129</v>
+      </c>
+      <c r="C20" s="6" t="s">
+        <v>130</v>
+      </c>
+      <c r="D20" s="6"/>
+    </row>
+    <row r="21" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A21" s="6"/>
+      <c r="B21" s="6" t="s">
+        <v>131</v>
+      </c>
+      <c r="C21" s="6" t="s">
+        <v>132</v>
+      </c>
+      <c r="D21" s="6"/>
+    </row>
+    <row r="22" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A22" s="6"/>
+      <c r="B22" s="6" t="s">
+        <v>133</v>
+      </c>
+      <c r="C22" s="6" t="s">
+        <v>134</v>
+      </c>
+      <c r="D22" s="6"/>
+    </row>
+    <row r="23" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A23" s="6"/>
+      <c r="B23" s="6" t="s">
+        <v>135</v>
+      </c>
+      <c r="C23" s="6" t="s">
+        <v>136</v>
+      </c>
+      <c r="D23" s="6"/>
+    </row>
+    <row r="24" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A24" s="9" t="s">
+        <v>137</v>
+      </c>
+      <c r="B24" s="6" t="s">
+        <v>138</v>
+      </c>
+      <c r="C24" s="6" t="s">
+        <v>139</v>
+      </c>
+      <c r="D24" s="6"/>
+    </row>
+    <row r="25" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A25" s="6"/>
+      <c r="B25" s="6" t="s">
+        <v>140</v>
+      </c>
+      <c r="C25" s="6" t="s">
+        <v>141</v>
+      </c>
+      <c r="D25" s="6"/>
+    </row>
+    <row r="26" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A26" s="6"/>
+      <c r="B26" s="6" t="s">
+        <v>142</v>
+      </c>
+      <c r="C26" s="6" t="s">
+        <v>143</v>
+      </c>
+      <c r="D26" s="6"/>
+    </row>
+    <row r="27" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A27" s="6"/>
+      <c r="B27" s="6" t="s">
+        <v>144</v>
+      </c>
+      <c r="C27" s="6" t="s">
+        <v>145</v>
+      </c>
+      <c r="D27" s="6"/>
+    </row>
+    <row r="28" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A28" s="6"/>
+      <c r="B28" s="6" t="s">
+        <v>146</v>
+      </c>
+      <c r="C28" s="6" t="s">
+        <v>147</v>
+      </c>
+      <c r="D28" s="6"/>
+    </row>
+    <row r="29" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A29" s="6"/>
+      <c r="B29" s="6" t="s">
+        <v>148</v>
+      </c>
+      <c r="C29" s="6" t="s">
+        <v>149</v>
+      </c>
+      <c r="D29" s="6"/>
+    </row>
+    <row r="30" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A30" s="6"/>
+      <c r="B30" s="6" t="s">
+        <v>150</v>
+      </c>
+      <c r="C30" s="6" t="s">
+        <v>151</v>
+      </c>
+      <c r="D30" s="6"/>
+    </row>
+    <row r="31" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A31" s="6"/>
+      <c r="B31" s="6" t="s">
+        <v>152</v>
+      </c>
+      <c r="C31" s="6" t="s">
+        <v>153</v>
+      </c>
+      <c r="D31" s="6"/>
+    </row>
+    <row r="32" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A32" s="6"/>
+      <c r="B32" s="6" t="s">
+        <v>154</v>
+      </c>
+      <c r="C32" s="6" t="s">
+        <v>155</v>
+      </c>
+      <c r="D32" s="6"/>
+    </row>
+    <row r="33" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A33" s="6"/>
+      <c r="B33" s="6" t="s">
+        <v>156</v>
+      </c>
+      <c r="C33" s="6" t="s">
+        <v>157</v>
+      </c>
+      <c r="D33" s="6"/>
+    </row>
+    <row r="34" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A34" s="10" t="s">
+        <v>158</v>
+      </c>
+      <c r="B34" s="6" t="s">
+        <v>159</v>
+      </c>
+      <c r="C34" s="6" t="s">
+        <v>160</v>
+      </c>
+      <c r="D34" s="6"/>
+    </row>
+    <row r="35" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A35" s="6"/>
+      <c r="B35" s="6" t="s">
+        <v>161</v>
+      </c>
+      <c r="C35" s="6" t="s">
+        <v>162</v>
+      </c>
+      <c r="D35" s="6"/>
+    </row>
+    <row r="36" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A36" s="6"/>
+      <c r="B36" s="6" t="s">
+        <v>163</v>
+      </c>
+      <c r="C36" s="6" t="s">
+        <v>164</v>
+      </c>
+      <c r="D36" s="6"/>
+    </row>
+    <row r="37" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A37" s="6"/>
+      <c r="B37" s="6" t="s">
+        <v>165</v>
+      </c>
+      <c r="C37" s="6" t="s">
+        <v>166</v>
+      </c>
+      <c r="D37" s="6"/>
+    </row>
+    <row r="38" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A38" s="6"/>
+      <c r="B38" s="6" t="s">
+        <v>167</v>
+      </c>
+      <c r="C38" s="6" t="s">
+        <v>168</v>
+      </c>
+      <c r="D38" s="6"/>
+    </row>
+    <row r="39" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A39" s="6"/>
+      <c r="B39" s="6" t="s">
+        <v>169</v>
+      </c>
+      <c r="C39" s="6" t="s">
+        <v>170</v>
+      </c>
+      <c r="D39" s="6"/>
+    </row>
+    <row r="40" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A40" s="6"/>
+      <c r="B40" s="6" t="s">
+        <v>171</v>
+      </c>
+      <c r="C40" s="6" t="s">
+        <v>172</v>
+      </c>
+      <c r="D40" s="6"/>
+    </row>
+    <row r="41" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A41" s="6"/>
+      <c r="B41" s="6" t="s">
+        <v>173</v>
+      </c>
+      <c r="C41" s="6" t="s">
+        <v>174</v>
+      </c>
+      <c r="D41" s="6"/>
+    </row>
+    <row r="42" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A42" s="6"/>
+      <c r="B42" s="6" t="s">
+        <v>7</v>
+      </c>
+      <c r="C42" s="6" t="s">
+        <v>175</v>
+      </c>
+      <c r="D42" s="6"/>
+    </row>
+    <row r="43" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A43" s="6"/>
+      <c r="B43" s="6" t="s">
+        <v>176</v>
+      </c>
+      <c r="C43" s="6" t="s">
+        <v>177</v>
+      </c>
+      <c r="D43" s="6"/>
+    </row>
+    <row r="44" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A44" s="11" t="s">
+        <v>178</v>
+      </c>
+      <c r="B44" s="6" t="s">
+        <v>179</v>
+      </c>
+      <c r="C44" s="6" t="s">
+        <v>180</v>
+      </c>
+      <c r="D44" s="6"/>
+    </row>
+    <row r="45" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A45" s="6"/>
+      <c r="B45" s="6" t="s">
+        <v>181</v>
+      </c>
+      <c r="C45" s="6" t="s">
+        <v>182</v>
+      </c>
+      <c r="D45" s="6"/>
+    </row>
+    <row r="46" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A46" s="6"/>
+      <c r="B46" s="5" t="s">
+        <v>183</v>
+      </c>
+      <c r="C46" s="6" t="s">
+        <v>184</v>
+      </c>
+      <c r="D46" s="6"/>
+    </row>
+    <row r="47" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A47" s="6"/>
+      <c r="B47" s="6" t="s">
+        <v>185</v>
+      </c>
+      <c r="C47" s="6" t="s">
+        <v>186</v>
+      </c>
+      <c r="D47" s="6"/>
+    </row>
+    <row r="48" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A48" s="6"/>
+      <c r="B48" s="6" t="s">
+        <v>187</v>
+      </c>
+      <c r="C48" s="6" t="s">
+        <v>188</v>
+      </c>
+      <c r="D48" s="6"/>
+    </row>
+    <row r="49" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A49" s="6"/>
+      <c r="B49" s="6" t="s">
+        <v>189</v>
+      </c>
+      <c r="C49" s="6" t="s">
+        <v>190</v>
+      </c>
+      <c r="D49" s="6"/>
+    </row>
+    <row r="50" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A50" s="6"/>
+      <c r="B50" s="6" t="s">
+        <v>191</v>
+      </c>
+      <c r="C50" s="6" t="s">
+        <v>192</v>
+      </c>
+      <c r="D50" s="6"/>
+    </row>
+    <row r="51" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A51" s="6"/>
+      <c r="B51" s="6" t="s">
+        <v>193</v>
+      </c>
+      <c r="C51" s="6" t="s">
+        <v>194</v>
+      </c>
+      <c r="D51" s="6"/>
+    </row>
+    <row r="52" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A52" s="6"/>
+      <c r="B52" s="6" t="s">
+        <v>195</v>
+      </c>
+      <c r="C52" s="6" t="s">
+        <v>196</v>
+      </c>
+      <c r="D52" s="6"/>
+    </row>
+    <row r="53" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A53" s="6"/>
+      <c r="B53" s="6" t="s">
+        <v>197</v>
+      </c>
+      <c r="C53" s="6" t="s">
+        <v>198</v>
+      </c>
+      <c r="D53" s="6"/>
+    </row>
+    <row r="54" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A54" s="12" t="s">
+        <v>199</v>
+      </c>
+      <c r="B54" s="6" t="s">
+        <v>200</v>
+      </c>
+      <c r="C54" s="6" t="s">
+        <v>201</v>
+      </c>
+      <c r="D54" s="6"/>
+    </row>
+    <row r="55" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A55" s="6"/>
+      <c r="B55" s="6" t="s">
+        <v>202</v>
+      </c>
+      <c r="C55" s="6" t="s">
+        <v>203</v>
+      </c>
+      <c r="D55" s="6"/>
+    </row>
+    <row r="56" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A56" s="6"/>
+      <c r="B56" s="6" t="s">
+        <v>204</v>
+      </c>
+      <c r="C56" s="6" t="s">
+        <v>205</v>
+      </c>
+      <c r="D56" s="6"/>
+    </row>
+    <row r="57" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A57" s="6"/>
+      <c r="B57" s="6" t="s">
+        <v>206</v>
+      </c>
+      <c r="C57" s="6" t="s">
+        <v>207</v>
+      </c>
+      <c r="D57" s="6"/>
+    </row>
+    <row r="58" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A58" s="6"/>
+      <c r="B58" s="6" t="s">
+        <v>208</v>
+      </c>
+      <c r="C58" s="6" t="s">
+        <v>209</v>
+      </c>
+      <c r="D58" s="6"/>
+    </row>
+    <row r="59" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A59" s="6"/>
+      <c r="B59" s="6" t="s">
+        <v>210</v>
+      </c>
+      <c r="C59" s="6" t="s">
+        <v>211</v>
+      </c>
+      <c r="D59" s="6"/>
+    </row>
+    <row r="60" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A60" s="13" t="s">
+        <v>212</v>
+      </c>
+      <c r="B60" s="6" t="s">
+        <v>213</v>
+      </c>
+      <c r="C60" s="6" t="s">
+        <v>214</v>
+      </c>
+      <c r="D60" s="6"/>
+    </row>
+    <row r="61" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A61" s="6"/>
+      <c r="B61" s="6" t="s">
+        <v>215</v>
+      </c>
+      <c r="C61" s="6" t="s">
+        <v>216</v>
+      </c>
+      <c r="D61" s="6"/>
+    </row>
+    <row r="62" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A62" s="6"/>
+      <c r="B62" s="6" t="s">
+        <v>217</v>
+      </c>
+      <c r="C62" s="6" t="s">
+        <v>218</v>
+      </c>
+      <c r="D62" s="6"/>
+    </row>
+    <row r="63" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A63" s="6"/>
+      <c r="B63" s="6" t="s">
+        <v>219</v>
+      </c>
+      <c r="C63" s="6" t="s">
+        <v>220</v>
+      </c>
+      <c r="D63" s="6"/>
+    </row>
+    <row r="64" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A64" s="6"/>
+      <c r="B64" s="6" t="s">
+        <v>221</v>
+      </c>
+      <c r="C64" s="6" t="s">
+        <v>222</v>
+      </c>
+      <c r="D64" s="6"/>
+    </row>
+    <row r="65" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A65" s="6"/>
+      <c r="B65" s="6" t="s">
+        <v>223</v>
+      </c>
+      <c r="C65" s="6" t="s">
+        <v>224</v>
+      </c>
+      <c r="D65" s="6"/>
+    </row>
+    <row r="66" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A66" s="6"/>
+      <c r="B66" s="6" t="s">
+        <v>225</v>
+      </c>
+      <c r="C66" s="6" t="s">
+        <v>226</v>
+      </c>
+      <c r="D66" s="6"/>
+    </row>
+    <row r="67" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A67" s="6"/>
+      <c r="B67" s="6" t="s">
+        <v>227</v>
+      </c>
+      <c r="C67" s="6" t="s">
+        <v>228</v>
+      </c>
+      <c r="D67" s="6"/>
+    </row>
+    <row r="68" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A68" s="6"/>
+      <c r="B68" s="6" t="s">
+        <v>229</v>
+      </c>
+      <c r="C68" s="6" t="s">
+        <v>230</v>
+      </c>
+      <c r="D68" s="6"/>
+    </row>
+    <row r="69" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A69" s="6"/>
+      <c r="B69" s="6" t="s">
+        <v>231</v>
+      </c>
+      <c r="C69" s="6" t="s">
+        <v>232</v>
+      </c>
+      <c r="D69" s="6"/>
+    </row>
+    <row r="70" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A70" s="6"/>
+      <c r="B70" s="6" t="s">
+        <v>233</v>
+      </c>
+      <c r="C70" s="6" t="s">
+        <v>234</v>
+      </c>
+      <c r="D70" s="6"/>
+    </row>
+    <row r="71" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A71" s="6"/>
+      <c r="B71" s="6" t="s">
+        <v>235</v>
+      </c>
+      <c r="C71" s="6" t="s">
+        <v>236</v>
+      </c>
+      <c r="D71" s="6"/>
+    </row>
+    <row r="72" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A72" s="6"/>
+      <c r="B72" s="6" t="s">
+        <v>237</v>
+      </c>
+      <c r="C72" s="6" t="s">
+        <v>238</v>
+      </c>
+      <c r="D72" s="6"/>
+    </row>
+    <row r="73" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A73" s="6"/>
+      <c r="B73" s="6" t="s">
+        <v>239</v>
+      </c>
+      <c r="C73" s="6" t="s">
+        <v>240</v>
+      </c>
+      <c r="D73" s="6"/>
+    </row>
+    <row r="74" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A74" s="6"/>
+      <c r="B74" s="6" t="s">
+        <v>241</v>
+      </c>
+      <c r="C74" s="6" t="s">
+        <v>242</v>
+      </c>
+      <c r="D74" s="6"/>
+    </row>
+    <row r="75" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A75" s="6"/>
+      <c r="B75" s="6" t="s">
+        <v>243</v>
+      </c>
+      <c r="C75" s="6" t="s">
+        <v>244</v>
+      </c>
+      <c r="D75" s="6"/>
+    </row>
+  </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
chore:data drivern added to tc3,tc4,tc5
</commit_message>
<xml_diff>
--- a/src/test/resources/CourseraAutomationData.xlsx
+++ b/src/test/resources/CourseraAutomationData.xlsx
@@ -45,7 +45,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="54" uniqueCount="42">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="70" uniqueCount="55">
   <si>
     <t>Search</t>
   </si>
@@ -171,6 +171,57 @@
   </si>
   <si>
     <t>Meta Web Development Fundamentals</t>
+  </si>
+  <si>
+    <t>https://www.coursera.org/partners/huji</t>
+  </si>
+  <si>
+    <t>true</t>
+  </si>
+  <si>
+    <t>Hebrew University of Jerusalem</t>
+  </si>
+  <si>
+    <t>https://www.coursera.org/partners/technion</t>
+  </si>
+  <si>
+    <t>Technion - Israel Institute of Technology</t>
+  </si>
+  <si>
+    <t>https://www.coursera.org/partners/telaviv</t>
+  </si>
+  <si>
+    <t>Tel Aviv University</t>
+  </si>
+  <si>
+    <t>https://www.coursera.org/partners/yadvashem</t>
+  </si>
+  <si>
+    <t>Yad Vashem</t>
+  </si>
+  <si>
+    <t>Indian Institute of Technology Guwahati
+Bachelor of Science in Data Science &amp; AI
+Named as one of the world’s top universities for the study of Data Science (QS World University Rankings by Subject 2024)
+Application due July 30, 2025</t>
+  </si>
+  <si>
+    <t>Birla Institute of Technology &amp; Science, Pilani
+Bachelor of Science in Computer Science
+Ranked #7 among Technical Universities in India (The Week-Hansa Research Best Universities Survey 2024)
+Application due August 3, 2025</t>
+  </si>
+  <si>
+    <t>University of London
+Bachelor of Science in Computer Science
+Specialise in ML and AI, data science, web and mobile development, physical computing and IoT, game development, VR, or UX
+Application due September 8, 2025</t>
+  </si>
+  <si>
+    <t>University of London
+International Foundation Programme for Computer Science
+Secure your future in computer science regardless of your academic or professional experience and qualifications
+Application due December 5, 2025</t>
   </si>
 </sst>
 </file>
@@ -811,7 +862,7 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4877FAC2-2A6B-46DD-8D6C-E52B161D8FA6}">
-  <dimension ref="A1:C1"/>
+  <dimension ref="A1:C5"/>
   <sheetViews>
     <sheetView topLeftCell="T1" workbookViewId="0">
       <selection activeCell="D11" sqref="D11"/>
@@ -835,6 +886,50 @@
         <v>17</v>
       </c>
     </row>
+    <row r="2">
+      <c r="A2" t="s" s="0">
+        <v>42</v>
+      </c>
+      <c r="B2" t="s" s="0">
+        <v>43</v>
+      </c>
+      <c r="C2" t="s" s="0">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" t="s" s="0">
+        <v>45</v>
+      </c>
+      <c r="B3" t="s" s="0">
+        <v>43</v>
+      </c>
+      <c r="C3" t="s" s="0">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" t="s" s="0">
+        <v>47</v>
+      </c>
+      <c r="B4" t="s" s="0">
+        <v>43</v>
+      </c>
+      <c r="C4" t="s" s="0">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" t="s" s="0">
+        <v>49</v>
+      </c>
+      <c r="B5" t="s" s="0">
+        <v>43</v>
+      </c>
+      <c r="C5" t="s" s="0">
+        <v>50</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -842,7 +937,7 @@
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{50AE5632-D04D-4B85-93F9-0760C2D5CD44}">
-  <dimension ref="A1"/>
+  <dimension ref="A1:A5"/>
   <sheetViews>
     <sheetView topLeftCell="S1" workbookViewId="0"/>
   </sheetViews>
@@ -854,6 +949,26 @@
     <row r="1" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A1" s="3" t="s">
         <v>18</v>
+      </c>
+    </row>
+    <row r="2">
+      <c r="A2" t="s" s="0">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" t="s" s="0">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" t="s" s="0">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" t="s" s="0">
+        <v>54</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
feat: Using Constants utility file for excel
</commit_message>
<xml_diff>
--- a/src/test/resources/CourseraAutomationData.xlsx
+++ b/src/test/resources/CourseraAutomationData.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Personal\Automation\workspace\CourseraAutomation\src\test\resources\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{32770861-166B-4F4B-BC5D-0934DBB9C330}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C141960F-AC4E-4CEB-9460-7371A094A874}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="4800" yWindow="0" windowWidth="14400" windowHeight="7270" xr2:uid="{8CA69206-0C49-4EFD-98F1-4AF42D798B8E}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" firstSheet="6" activeTab="6" xr2:uid="{8CA69206-0C49-4EFD-98F1-4AF42D798B8E}"/>
   </bookViews>
   <sheets>
     <sheet name="CourseDetails" sheetId="1" r:id="rId1"/>
@@ -45,7 +45,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="54" uniqueCount="42">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="289" uniqueCount="267">
   <si>
     <t>Search</t>
   </si>
@@ -77,9 +77,6 @@
     <t>Beginner</t>
   </si>
   <si>
-    <t>Available Course</t>
-  </si>
-  <si>
     <t>Country Name</t>
   </si>
   <si>
@@ -171,6 +168,684 @@
   </si>
   <si>
     <t>Meta Web Development Fundamentals</t>
+  </si>
+  <si>
+    <t>No of Course</t>
+  </si>
+  <si>
+    <t>Italian</t>
+  </si>
+  <si>
+    <t>2156</t>
+  </si>
+  <si>
+    <t>Russian</t>
+  </si>
+  <si>
+    <t>2237</t>
+  </si>
+  <si>
+    <t>Uzbek</t>
+  </si>
+  <si>
+    <t>514</t>
+  </si>
+  <si>
+    <t>Hebrew</t>
+  </si>
+  <si>
+    <t>5</t>
+  </si>
+  <si>
+    <t>German</t>
+  </si>
+  <si>
+    <t>2328</t>
+  </si>
+  <si>
+    <t>Turkish</t>
+  </si>
+  <si>
+    <t>2168</t>
+  </si>
+  <si>
+    <t>Swedish</t>
+  </si>
+  <si>
+    <t>2129</t>
+  </si>
+  <si>
+    <t>Azerbaijani</t>
+  </si>
+  <si>
+    <t>459</t>
+  </si>
+  <si>
+    <t>Ukrainian</t>
+  </si>
+  <si>
+    <t>2166</t>
+  </si>
+  <si>
+    <t>Arabic</t>
+  </si>
+  <si>
+    <t>2485</t>
+  </si>
+  <si>
+    <t>French</t>
+  </si>
+  <si>
+    <t>2459</t>
+  </si>
+  <si>
+    <t>Portuguese</t>
+  </si>
+  <si>
+    <t>1</t>
+  </si>
+  <si>
+    <t>Chinese (Traditional)</t>
+  </si>
+  <si>
+    <t>42</t>
+  </si>
+  <si>
+    <t>Indonesian</t>
+  </si>
+  <si>
+    <t>2301</t>
+  </si>
+  <si>
+    <t>Chinese (China)</t>
+  </si>
+  <si>
+    <t>2329</t>
+  </si>
+  <si>
+    <t>Catalan</t>
+  </si>
+  <si>
+    <t>Spanish</t>
+  </si>
+  <si>
+    <t>2969</t>
+  </si>
+  <si>
+    <t>Hindi</t>
+  </si>
+  <si>
+    <t>2211</t>
+  </si>
+  <si>
+    <t>Thai</t>
+  </si>
+  <si>
+    <t>2142</t>
+  </si>
+  <si>
+    <t>Pushto</t>
+  </si>
+  <si>
+    <t>254</t>
+  </si>
+  <si>
+    <t>Portuguese (Portugal)</t>
+  </si>
+  <si>
+    <t>Polish</t>
+  </si>
+  <si>
+    <t>2135</t>
+  </si>
+  <si>
+    <t>Korean</t>
+  </si>
+  <si>
+    <t>Japanese</t>
+  </si>
+  <si>
+    <t>Croatian</t>
+  </si>
+  <si>
+    <t>6239</t>
+  </si>
+  <si>
+    <t>Kazakh</t>
+  </si>
+  <si>
+    <t>1977</t>
+  </si>
+  <si>
+    <t>Vietnamese</t>
+  </si>
+  <si>
+    <t>484</t>
+  </si>
+  <si>
+    <t>Hungarian</t>
+  </si>
+  <si>
+    <t>1354</t>
+  </si>
+  <si>
+    <t>Dutch</t>
+  </si>
+  <si>
+    <t>2132</t>
+  </si>
+  <si>
+    <t>Greek</t>
+  </si>
+  <si>
+    <t>2130</t>
+  </si>
+  <si>
+    <t>Portuguese (Brazil)</t>
+  </si>
+  <si>
+    <t>2431</t>
+  </si>
+  <si>
+    <t>4 modules</t>
+  </si>
+  <si>
+    <t>(530 reviews)</t>
+  </si>
+  <si>
+    <t>Scripting</t>
+  </si>
+  <si>
+    <t>Bootstrap (Front-End Framework)</t>
+  </si>
+  <si>
+    <t>Application Programming Interface (API)</t>
+  </si>
+  <si>
+    <t>Cascading Style Sheets (CSS)</t>
+  </si>
+  <si>
+    <t>Responsive Web Design</t>
+  </si>
+  <si>
+    <t>Browser Compatibility</t>
+  </si>
+  <si>
+    <t>Javascript</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Describe the Web Application Development Ecosystem and terminology like front-end developer, back-end, server-side, and full stack. </t>
+  </si>
+  <si>
+    <t>Identify the developer tools, online editors like JSFiddle, and integrated development environments (IDEs) for building and testing web applications.</t>
+  </si>
+  <si>
+    <t>Create and structure basic web pages using HTML and style them with CSS.</t>
+  </si>
+  <si>
+    <t>Develop dynamic and interactive web pages using JavaScript, including DOM manipulation, form validation, and client-side scripting techniques.</t>
+  </si>
+  <si>
+    <t>More</t>
+  </si>
+  <si>
+    <t>Privacy</t>
+  </si>
+  <si>
+    <t>https://www.coursera.org/about/privacy</t>
+  </si>
+  <si>
+    <t>Manage Cookie Preferences</t>
+  </si>
+  <si>
+    <t>https://www.coursera.org/about/cookies-manage</t>
+  </si>
+  <si>
+    <t>Investors</t>
+  </si>
+  <si>
+    <t>https://investor.coursera.com/</t>
+  </si>
+  <si>
+    <t>Help</t>
+  </si>
+  <si>
+    <t>https://learner.coursera.help/hc</t>
+  </si>
+  <si>
+    <t>Accessibility</t>
+  </si>
+  <si>
+    <t>https://learner.coursera.help/hc/articles/360050668591-Accessibility-Statement</t>
+  </si>
+  <si>
+    <t>Articles</t>
+  </si>
+  <si>
+    <t>https://www.coursera.org/articles</t>
+  </si>
+  <si>
+    <t>Modern Slavery Statement</t>
+  </si>
+  <si>
+    <t>https://coursera_assets.s3.amazonaws.com/footer/Modern+Slavery+Statement+(approved+March+26%2C+2025).pdf</t>
+  </si>
+  <si>
+    <t>Affiliates</t>
+  </si>
+  <si>
+    <t>https://about.coursera.org/affiliates</t>
+  </si>
+  <si>
+    <t>Terms</t>
+  </si>
+  <si>
+    <t>https://www.coursera.org/about/terms</t>
+  </si>
+  <si>
+    <t>Press</t>
+  </si>
+  <si>
+    <t>https://www.coursera.org/about/press</t>
+  </si>
+  <si>
+    <t>Contact</t>
+  </si>
+  <si>
+    <t>https://www.coursera.org/about/contact</t>
+  </si>
+  <si>
+    <t>Directory</t>
+  </si>
+  <si>
+    <t>https://www.coursera.org/directory</t>
+  </si>
+  <si>
+    <t>Career Resources</t>
+  </si>
+  <si>
+    <t>How to Learn Artificial Intelligence</t>
+  </si>
+  <si>
+    <t>https://www.coursera.org/articles/how-to-learn-artificial-intelligence</t>
+  </si>
+  <si>
+    <t>Share your Coursera Learning Story</t>
+  </si>
+  <si>
+    <t>https://airtable.com/appxSsG2Dz9CjSpF8/pagCDDP2Uinw59CNP/form</t>
+  </si>
+  <si>
+    <t>Popular Cybersecurity Certifications</t>
+  </si>
+  <si>
+    <t>https://www.coursera.org/articles/popular-cybersecurity-certifications</t>
+  </si>
+  <si>
+    <t>How to Get a PMP Certification</t>
+  </si>
+  <si>
+    <t>https://www.coursera.org/articles/the-pmp-certification-a-guide-to-getting-started</t>
+  </si>
+  <si>
+    <t>Career Aptitude Test</t>
+  </si>
+  <si>
+    <t>https://www.coursera.org/resources/career-quiz</t>
+  </si>
+  <si>
+    <t>Career Development Resources</t>
+  </si>
+  <si>
+    <t>https://www.coursera.org/resources</t>
+  </si>
+  <si>
+    <t>Popular Data Analytics Certifications</t>
+  </si>
+  <si>
+    <t>https://www.coursera.org/articles/data-analytics-certification</t>
+  </si>
+  <si>
+    <t>Essential IT Certifications</t>
+  </si>
+  <si>
+    <t>https://www.coursera.org/articles/essential-it-certifications-entry-level-and-beginner</t>
+  </si>
+  <si>
+    <t>What Does a Data Analyst Do?</t>
+  </si>
+  <si>
+    <t>https://www.coursera.org/articles/what-does-a-data-analyst-do-a-career-guide</t>
+  </si>
+  <si>
+    <t>High-Income Skills to Learn</t>
+  </si>
+  <si>
+    <t>https://www.coursera.org/articles/high-income-skills</t>
+  </si>
+  <si>
+    <t>Analytical Skills</t>
+  </si>
+  <si>
+    <t>Data Science</t>
+  </si>
+  <si>
+    <t>https://www.coursera.org/courses?query=data%20science&amp;topic=Data%20Science</t>
+  </si>
+  <si>
+    <t>Artificial Intelligence</t>
+  </si>
+  <si>
+    <t>https://www.coursera.org/courses?query=artificial%20intelligence</t>
+  </si>
+  <si>
+    <t>Microsoft Power BI</t>
+  </si>
+  <si>
+    <t>https://www.coursera.org/courses?query=microsoft%20power%20bi</t>
+  </si>
+  <si>
+    <t>Big Data</t>
+  </si>
+  <si>
+    <t>https://www.coursera.org/courses?query=big%20data</t>
+  </si>
+  <si>
+    <t>Financial Modeling</t>
+  </si>
+  <si>
+    <t>https://www.coursera.org/courses?query=financial%20modeling</t>
+  </si>
+  <si>
+    <t>Data Analytics</t>
+  </si>
+  <si>
+    <t>https://www.coursera.org/courses?query=data%20analytics</t>
+  </si>
+  <si>
+    <t>Machine Learning</t>
+  </si>
+  <si>
+    <t>https://www.coursera.org/courses?query=machine%20learning&amp;skills=Machine%20Learning</t>
+  </si>
+  <si>
+    <t>Microsoft Excel</t>
+  </si>
+  <si>
+    <t>https://www.coursera.org/courses?query=microsoft%20excel</t>
+  </si>
+  <si>
+    <t>Business Analysis</t>
+  </si>
+  <si>
+    <t>https://www.coursera.org/courses?query=business%20analysis</t>
+  </si>
+  <si>
+    <t>SQL</t>
+  </si>
+  <si>
+    <t>https://www.coursera.org/courses?query=sql</t>
+  </si>
+  <si>
+    <t>Technical Skills</t>
+  </si>
+  <si>
+    <t>Ethical Hacking</t>
+  </si>
+  <si>
+    <t>https://www.coursera.org/courses?query=ethical%20hacking</t>
+  </si>
+  <si>
+    <t>DevOps</t>
+  </si>
+  <si>
+    <t>https://www.coursera.org/courses?query=devops</t>
+  </si>
+  <si>
+    <t>Generative AI</t>
+  </si>
+  <si>
+    <t>https://www.coursera.org/courses?query=generative%20ai</t>
+  </si>
+  <si>
+    <t>ChatGPT</t>
+  </si>
+  <si>
+    <t>https://www.coursera.org/courses?query=chatgpt</t>
+  </si>
+  <si>
+    <t>Coding</t>
+  </si>
+  <si>
+    <t>https://www.coursera.org/courses?query=coding</t>
+  </si>
+  <si>
+    <t>Computer Science</t>
+  </si>
+  <si>
+    <t>https://www.coursera.org/courses?query=computer%20science&amp;topic=Computer%20Science</t>
+  </si>
+  <si>
+    <t>Java Programming</t>
+  </si>
+  <si>
+    <t>https://www.coursera.org/courses?query=java</t>
+  </si>
+  <si>
+    <t>Cybersecurity</t>
+  </si>
+  <si>
+    <t>https://www.coursera.org/courses?query=cybersecurity</t>
+  </si>
+  <si>
+    <t>https://www.coursera.org/courses?query=web%20development</t>
+  </si>
+  <si>
+    <t>Python</t>
+  </si>
+  <si>
+    <t>https://www.coursera.org/courses?query=python</t>
+  </si>
+  <si>
+    <t>Business Skills</t>
+  </si>
+  <si>
+    <t>Google</t>
+  </si>
+  <si>
+    <t>https://www.coursera.org/courses?query=google</t>
+  </si>
+  <si>
+    <t>Project Management</t>
+  </si>
+  <si>
+    <t>https://www.coursera.org/courses?query=project%20management</t>
+  </si>
+  <si>
+    <t>Accounting</t>
+  </si>
+  <si>
+    <t>https://www.coursera.org/courses?query=accounting</t>
+  </si>
+  <si>
+    <t>IBM</t>
+  </si>
+  <si>
+    <t>https://www.coursera.org/courses?query=ibm</t>
+  </si>
+  <si>
+    <t>Finance</t>
+  </si>
+  <si>
+    <t>https://www.coursera.org/courses?query=finance&amp;skills=Finance</t>
+  </si>
+  <si>
+    <t>E-commerce</t>
+  </si>
+  <si>
+    <t>https://www.coursera.org/courses?query=e-commerce</t>
+  </si>
+  <si>
+    <t>Digital Marketing</t>
+  </si>
+  <si>
+    <t>https://www.coursera.org/courses?query=digital%20marketing</t>
+  </si>
+  <si>
+    <t>Social Media Marketing</t>
+  </si>
+  <si>
+    <t>https://www.coursera.org/courses?query=social%20media%20marketing</t>
+  </si>
+  <si>
+    <t>Graphic Design</t>
+  </si>
+  <si>
+    <t>https://www.coursera.org/courses?query=graphic%20design</t>
+  </si>
+  <si>
+    <t>Marketing</t>
+  </si>
+  <si>
+    <t>https://www.coursera.org/courses?query=marketing&amp;skills=Marketing</t>
+  </si>
+  <si>
+    <t>Community</t>
+  </si>
+  <si>
+    <t>Partners</t>
+  </si>
+  <si>
+    <t>https://www.coursera.org/partners</t>
+  </si>
+  <si>
+    <t>Tech Blog</t>
+  </si>
+  <si>
+    <t>https://medium.com/coursera-engineering</t>
+  </si>
+  <si>
+    <t>The Coursera Podcast</t>
+  </si>
+  <si>
+    <t>https://open.spotify.com/show/58M36bneU7REOofdPZxe6A</t>
+  </si>
+  <si>
+    <t>Beta Testers</t>
+  </si>
+  <si>
+    <t>https://www.coursera.support/s/article/360000152926-Become-a-Coursera-beta-tester</t>
+  </si>
+  <si>
+    <t>Learners</t>
+  </si>
+  <si>
+    <t>https://www.coursera.community/</t>
+  </si>
+  <si>
+    <t>Blog</t>
+  </si>
+  <si>
+    <t>https://blog.coursera.org/</t>
+  </si>
+  <si>
+    <t>Coursera</t>
+  </si>
+  <si>
+    <t>MasterTrack® Certificates</t>
+  </si>
+  <si>
+    <t>https://www.coursera.org/mastertrack</t>
+  </si>
+  <si>
+    <t>Leadership</t>
+  </si>
+  <si>
+    <t>https://about.coursera.org/leadership</t>
+  </si>
+  <si>
+    <t>Coursera Plus</t>
+  </si>
+  <si>
+    <t>https://www.coursera.org/courseraplus</t>
+  </si>
+  <si>
+    <t>Degrees</t>
+  </si>
+  <si>
+    <t>https://www.coursera.org/degrees</t>
+  </si>
+  <si>
+    <t>Become a Partner</t>
+  </si>
+  <si>
+    <t>https://partnerships.coursera.org/?utm_medium=coursera&amp;utm_source=partnerships&amp;utm_campaign=website&amp;utm_content=corp-to-home-footer-become-a-partner</t>
+  </si>
+  <si>
+    <t>For Enterprise</t>
+  </si>
+  <si>
+    <t>https://www.coursera.org/business?utm_campaign=website&amp;utm_content=corp-to-home-footer-for-enterprise&amp;utm_medium=coursera&amp;utm_source=enterprise</t>
+  </si>
+  <si>
+    <t>Careers</t>
+  </si>
+  <si>
+    <t>https://careers.coursera.com/</t>
+  </si>
+  <si>
+    <t>Professional Certificates</t>
+  </si>
+  <si>
+    <t>https://www.coursera.org/professional-certificate</t>
+  </si>
+  <si>
+    <t>What We Offer</t>
+  </si>
+  <si>
+    <t>https://about.coursera.org/how-coursera-works/</t>
+  </si>
+  <si>
+    <t>Catalog</t>
+  </si>
+  <si>
+    <t>https://www.coursera.org/browse</t>
+  </si>
+  <si>
+    <t>About</t>
+  </si>
+  <si>
+    <t>https://about.coursera.org/</t>
+  </si>
+  <si>
+    <t>For Government</t>
+  </si>
+  <si>
+    <t>https://www.coursera.org/government?utm_campaign=website&amp;utm_content=corp-to-home-footer-for-government&amp;utm_medium=coursera&amp;utm_source=enterprise</t>
+  </si>
+  <si>
+    <t>Social Impact</t>
+  </si>
+  <si>
+    <t>https://www.coursera.org/social-impact</t>
+  </si>
+  <si>
+    <t>ECTS Credit Recommendations</t>
+  </si>
+  <si>
+    <t>https://www.coursera.org/explore/ects-credit-recommendation</t>
+  </si>
+  <si>
+    <t>For Campus</t>
+  </si>
+  <si>
+    <t>https://www.coursera.org/campus?utm_campaign=website&amp;utm_content=corp-to-home-footer-for-campus&amp;utm_medium=coursera&amp;utm_source=enterprise</t>
+  </si>
+  <si>
+    <t>Free Courses</t>
+  </si>
+  <si>
+    <t>https://www.coursera.org/courses?query=free</t>
   </si>
 </sst>
 </file>
@@ -187,7 +862,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="5">
+  <fills count="7">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -210,6 +885,16 @@
       <patternFill patternType="solid">
         <fgColor theme="7" tint="0.39997558519241921"/>
         <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <fgColor indexed="17"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor indexed="17"/>
       </patternFill>
     </fill>
   </fills>
@@ -266,7 +951,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="10">
+  <cellXfs count="17">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
@@ -277,6 +962,13 @@
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFill="true"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -613,8 +1305,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7F790D43-1548-4D2B-B16C-E961EBAC6C05}">
   <dimension ref="A1:G7"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E2" sqref="E2:G7"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="E9" sqref="E9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -663,68 +1355,68 @@
         <v>6</v>
       </c>
       <c r="E2" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="F2" s="1" t="s">
         <v>30</v>
       </c>
-      <c r="F2" s="1" t="s">
+      <c r="G2" s="1" t="s">
         <v>31</v>
       </c>
-      <c r="G2" s="1" t="s">
+    </row>
+    <row r="3" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="E3" t="s" s="0">
         <v>32</v>
       </c>
-    </row>
-    <row r="3">
-      <c r="E3" t="s" s="0">
+      <c r="F3" t="s" s="0">
         <v>33</v>
       </c>
-      <c r="F3" t="s" s="0">
+      <c r="G3" t="s" s="0">
         <v>34</v>
       </c>
-      <c r="G3" t="s" s="0">
+    </row>
+    <row r="4" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="E4" t="s" s="0">
         <v>35</v>
       </c>
-    </row>
-    <row r="4">
-      <c r="E4" t="s" s="0">
+      <c r="F4" t="s" s="0">
+        <v>30</v>
+      </c>
+      <c r="G4" t="s" s="0">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="5" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="E5" t="s" s="0">
         <v>36</v>
       </c>
-      <c r="F4" t="s" s="0">
+      <c r="F5" t="s" s="0">
+        <v>37</v>
+      </c>
+      <c r="G5" t="s" s="0">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="6" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="E6" t="s" s="0">
+        <v>39</v>
+      </c>
+      <c r="F6" t="s" s="0">
+        <v>30</v>
+      </c>
+      <c r="G6" t="s" s="0">
         <v>31</v>
       </c>
-      <c r="G4" t="s" s="0">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="5">
-      <c r="E5" t="s" s="0">
-        <v>37</v>
-      </c>
-      <c r="F5" t="s" s="0">
-        <v>38</v>
-      </c>
-      <c r="G5" t="s" s="0">
-        <v>39</v>
-      </c>
-    </row>
-    <row r="6">
-      <c r="E6" t="s" s="0">
+    </row>
+    <row r="7" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="E7" t="s" s="0">
         <v>40</v>
       </c>
-      <c r="F6" t="s" s="0">
+      <c r="F7" t="s" s="0">
+        <v>30</v>
+      </c>
+      <c r="G7" t="s" s="0">
         <v>31</v>
-      </c>
-      <c r="G6" t="s" s="0">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="7">
-      <c r="E7" t="s" s="0">
-        <v>41</v>
-      </c>
-      <c r="F7" t="s" s="0">
-        <v>31</v>
-      </c>
-      <c r="G7" t="s" s="0">
-        <v>32</v>
       </c>
     </row>
   </sheetData>
@@ -746,10 +1438,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{EF702DC1-638B-4A54-99C8-3AD2DDCC37F1}">
-  <dimension ref="A1:B1"/>
+  <dimension ref="A1:B33"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B1" sqref="A1:B1"/>
+      <selection activeCell="B1" sqref="B1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -763,7 +1455,263 @@
         <v>1</v>
       </c>
       <c r="B1" s="9" t="s">
-        <v>10</v>
+        <v>41</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A2" t="s" s="0">
+        <v>42</v>
+      </c>
+      <c r="B2" t="s" s="0">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A3" t="s" s="0">
+        <v>44</v>
+      </c>
+      <c r="B3" t="s" s="0">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A4" t="s" s="0">
+        <v>46</v>
+      </c>
+      <c r="B4" t="s" s="0">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A5" t="s" s="0">
+        <v>48</v>
+      </c>
+      <c r="B5" t="s" s="0">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A6" t="s" s="0">
+        <v>50</v>
+      </c>
+      <c r="B6" t="s" s="0">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A7" t="s" s="0">
+        <v>52</v>
+      </c>
+      <c r="B7" t="s" s="0">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="8" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A8" t="s" s="0">
+        <v>54</v>
+      </c>
+      <c r="B8" t="s" s="0">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="9" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A9" t="s" s="0">
+        <v>56</v>
+      </c>
+      <c r="B9" t="s" s="0">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="10" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A10" t="s" s="0">
+        <v>58</v>
+      </c>
+      <c r="B10" t="s" s="0">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="11" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A11" t="s" s="0">
+        <v>60</v>
+      </c>
+      <c r="B11" t="s" s="0">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="12" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A12" t="s" s="0">
+        <v>62</v>
+      </c>
+      <c r="B12" t="s" s="0">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="13" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A13" t="s" s="0">
+        <v>64</v>
+      </c>
+      <c r="B13" t="s" s="0">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="14" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A14" t="s" s="0">
+        <v>66</v>
+      </c>
+      <c r="B14" t="s" s="0">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="15" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A15" t="s" s="0">
+        <v>68</v>
+      </c>
+      <c r="B15" t="s" s="0">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="16" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A16" t="s" s="0">
+        <v>70</v>
+      </c>
+      <c r="B16" t="s" s="0">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="17" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A17" t="s" s="0">
+        <v>72</v>
+      </c>
+      <c r="B17" t="s" s="0">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="18" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A18" t="s" s="0">
+        <v>73</v>
+      </c>
+      <c r="B18" t="s" s="0">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="19" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A19" t="s" s="0">
+        <v>75</v>
+      </c>
+      <c r="B19" t="s" s="0">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="20" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A20" t="s" s="0">
+        <v>77</v>
+      </c>
+      <c r="B20" t="s" s="0">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="21" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A21" t="s" s="0">
+        <v>79</v>
+      </c>
+      <c r="B21" t="s" s="0">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="22" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A22" t="s" s="0">
+        <v>81</v>
+      </c>
+      <c r="B22" t="s" s="0">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="23" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A23" t="s" s="0">
+        <v>82</v>
+      </c>
+      <c r="B23" t="s" s="0">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="24" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A24" t="s" s="0">
+        <v>84</v>
+      </c>
+      <c r="B24" t="s" s="0">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="25" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A25" t="s" s="0">
+        <v>85</v>
+      </c>
+      <c r="B25" t="s" s="0">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="26" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A26" t="s" s="0">
+        <v>86</v>
+      </c>
+      <c r="B26" t="s" s="0">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="27" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A27" t="s" s="0">
+        <v>8</v>
+      </c>
+      <c r="B27" t="s" s="0">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="28" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A28" t="s" s="0">
+        <v>88</v>
+      </c>
+      <c r="B28" t="s" s="0">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="29" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A29" t="s" s="0">
+        <v>90</v>
+      </c>
+      <c r="B29" t="s" s="0">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="30" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A30" t="s" s="0">
+        <v>92</v>
+      </c>
+      <c r="B30" t="s" s="0">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="31" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A31" t="s" s="0">
+        <v>94</v>
+      </c>
+      <c r="B31" t="s" s="0">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="32" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A32" t="s" s="0">
+        <v>96</v>
+      </c>
+      <c r="B32" t="s" s="0">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="33" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A33" t="s" s="0">
+        <v>98</v>
+      </c>
+      <c r="B33" t="s" s="0">
+        <v>99</v>
       </c>
     </row>
   </sheetData>
@@ -788,18 +1736,18 @@
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A1" s="5" t="s">
+        <v>10</v>
+      </c>
+      <c r="B1" s="3" t="s">
         <v>11</v>
       </c>
-      <c r="B1" s="3" t="s">
+      <c r="C1" s="3" t="s">
         <v>12</v>
-      </c>
-      <c r="C1" s="3" t="s">
-        <v>13</v>
       </c>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A2" s="4" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="B2" s="6"/>
       <c r="C2" s="6"/>
@@ -826,13 +1774,13 @@
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A1" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="B1" s="3" t="s">
         <v>15</v>
       </c>
-      <c r="B1" s="3" t="s">
+      <c r="C1" s="3" t="s">
         <v>16</v>
-      </c>
-      <c r="C1" s="3" t="s">
-        <v>17</v>
       </c>
     </row>
   </sheetData>
@@ -853,7 +1801,7 @@
   <sheetData>
     <row r="1" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A1" s="3" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
     </row>
   </sheetData>
@@ -876,13 +1824,13 @@
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A1" s="7" t="s">
+        <v>18</v>
+      </c>
+      <c r="B1" s="7" t="s">
         <v>19</v>
       </c>
-      <c r="B1" s="7" t="s">
+      <c r="C1" s="8" t="s">
         <v>20</v>
-      </c>
-      <c r="C1" s="8" t="s">
-        <v>21</v>
       </c>
     </row>
   </sheetData>
@@ -892,10 +1840,10 @@
 
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C731EF70-8147-435C-A429-F5FA1E52B0A3}">
-  <dimension ref="A1:G1"/>
+  <dimension ref="A1:G9"/>
   <sheetViews>
-    <sheetView topLeftCell="G1" workbookViewId="0">
-      <selection sqref="A1:G1"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -908,25 +1856,92 @@
   <sheetData>
     <row r="1" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A1" t="s" s="0">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="B1" t="s" s="0">
         <v>4</v>
       </c>
       <c r="C1" t="s" s="0">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="D1" t="s" s="0">
         <v>5</v>
       </c>
       <c r="E1" t="s" s="0">
+        <v>23</v>
+      </c>
+      <c r="F1" t="s" s="0">
         <v>24</v>
       </c>
-      <c r="F1" t="s" s="0">
+      <c r="G1" t="s" s="0">
         <v>25</v>
       </c>
-      <c r="G1" t="s" s="0">
-        <v>26</v>
+    </row>
+    <row r="2" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A2" s="0">
+        <v>1</v>
+      </c>
+      <c r="B2" t="s" s="0">
+        <v>32</v>
+      </c>
+      <c r="C2" t="s" s="0">
+        <v>100</v>
+      </c>
+      <c r="D2" t="s" s="0">
+        <v>33</v>
+      </c>
+      <c r="E2" t="s" s="0">
+        <v>101</v>
+      </c>
+      <c r="F2" t="s" s="0">
+        <v>102</v>
+      </c>
+      <c r="G2" t="s" s="0">
+        <v>109</v>
+      </c>
+    </row>
+    <row r="3">
+      <c r="F3" t="s" s="0">
+        <v>103</v>
+      </c>
+      <c r="G3" t="s" s="0">
+        <v>110</v>
+      </c>
+    </row>
+    <row r="4">
+      <c r="F4" t="s" s="0">
+        <v>104</v>
+      </c>
+      <c r="G4" t="s" s="0">
+        <v>111</v>
+      </c>
+    </row>
+    <row r="5">
+      <c r="F5" t="s" s="0">
+        <v>105</v>
+      </c>
+      <c r="G5" t="s" s="0">
+        <v>112</v>
+      </c>
+    </row>
+    <row r="6">
+      <c r="F6" t="s" s="0">
+        <v>106</v>
+      </c>
+    </row>
+    <row r="7">
+      <c r="F7" t="s" s="0">
+        <v>107</v>
+      </c>
+    </row>
+    <row r="8">
+      <c r="F8" t="s" s="0">
+        <v>108</v>
+      </c>
+    </row>
+    <row r="9">
+      <c r="F9" t="s" s="0">
+        <v>7</v>
       </c>
     </row>
   </sheetData>
@@ -955,15 +1970,15 @@
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A1" s="5" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="B1" s="8" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A2" s="4" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
     </row>
   </sheetData>
@@ -973,7 +1988,7 @@
 
 <file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8A3EB322-FF18-442E-8BCD-C9A28A47FC30}">
-  <dimension ref="A1:C1"/>
+  <dimension ref="A1:C75"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -981,13 +1996,626 @@
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A1" t="s" s="0">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="B1" t="s" s="0">
         <v>4</v>
       </c>
       <c r="C1" t="s" s="0">
-        <v>28</v>
+        <v>27</v>
+      </c>
+    </row>
+    <row r="2">
+      <c r="A2" t="s" s="10">
+        <v>113</v>
+      </c>
+      <c r="B2" t="s" s="0">
+        <v>114</v>
+      </c>
+      <c r="C2" t="s" s="0">
+        <v>115</v>
+      </c>
+    </row>
+    <row r="3">
+      <c r="B3" t="s" s="0">
+        <v>116</v>
+      </c>
+      <c r="C3" t="s" s="0">
+        <v>117</v>
+      </c>
+    </row>
+    <row r="4">
+      <c r="B4" t="s" s="0">
+        <v>118</v>
+      </c>
+      <c r="C4" t="s" s="0">
+        <v>119</v>
+      </c>
+    </row>
+    <row r="5">
+      <c r="B5" t="s" s="0">
+        <v>120</v>
+      </c>
+      <c r="C5" t="s" s="0">
+        <v>121</v>
+      </c>
+    </row>
+    <row r="6">
+      <c r="B6" t="s" s="0">
+        <v>122</v>
+      </c>
+      <c r="C6" t="s" s="0">
+        <v>123</v>
+      </c>
+    </row>
+    <row r="7">
+      <c r="B7" t="s" s="0">
+        <v>124</v>
+      </c>
+      <c r="C7" t="s" s="0">
+        <v>125</v>
+      </c>
+    </row>
+    <row r="8">
+      <c r="B8" t="s" s="0">
+        <v>126</v>
+      </c>
+      <c r="C8" t="s" s="0">
+        <v>127</v>
+      </c>
+    </row>
+    <row r="9">
+      <c r="B9" t="s" s="0">
+        <v>128</v>
+      </c>
+      <c r="C9" t="s" s="0">
+        <v>129</v>
+      </c>
+    </row>
+    <row r="10">
+      <c r="B10" t="s" s="0">
+        <v>130</v>
+      </c>
+      <c r="C10" t="s" s="0">
+        <v>131</v>
+      </c>
+    </row>
+    <row r="11">
+      <c r="B11" t="s" s="0">
+        <v>132</v>
+      </c>
+      <c r="C11" t="s" s="0">
+        <v>133</v>
+      </c>
+    </row>
+    <row r="12">
+      <c r="B12" t="s" s="0">
+        <v>134</v>
+      </c>
+      <c r="C12" t="s" s="0">
+        <v>135</v>
+      </c>
+    </row>
+    <row r="13">
+      <c r="B13" t="s" s="0">
+        <v>136</v>
+      </c>
+      <c r="C13" t="s" s="0">
+        <v>137</v>
+      </c>
+    </row>
+    <row r="14">
+      <c r="A14" t="s" s="11">
+        <v>138</v>
+      </c>
+      <c r="B14" t="s" s="0">
+        <v>139</v>
+      </c>
+      <c r="C14" t="s" s="0">
+        <v>140</v>
+      </c>
+    </row>
+    <row r="15">
+      <c r="B15" t="s" s="0">
+        <v>141</v>
+      </c>
+      <c r="C15" t="s" s="0">
+        <v>142</v>
+      </c>
+    </row>
+    <row r="16">
+      <c r="B16" t="s" s="0">
+        <v>143</v>
+      </c>
+      <c r="C16" t="s" s="0">
+        <v>144</v>
+      </c>
+    </row>
+    <row r="17">
+      <c r="B17" t="s" s="0">
+        <v>145</v>
+      </c>
+      <c r="C17" t="s" s="0">
+        <v>146</v>
+      </c>
+    </row>
+    <row r="18">
+      <c r="B18" t="s" s="0">
+        <v>147</v>
+      </c>
+      <c r="C18" t="s" s="0">
+        <v>148</v>
+      </c>
+    </row>
+    <row r="19">
+      <c r="B19" t="s" s="0">
+        <v>149</v>
+      </c>
+      <c r="C19" t="s" s="0">
+        <v>150</v>
+      </c>
+    </row>
+    <row r="20">
+      <c r="B20" t="s" s="0">
+        <v>151</v>
+      </c>
+      <c r="C20" t="s" s="0">
+        <v>152</v>
+      </c>
+    </row>
+    <row r="21">
+      <c r="B21" t="s" s="0">
+        <v>153</v>
+      </c>
+      <c r="C21" t="s" s="0">
+        <v>154</v>
+      </c>
+    </row>
+    <row r="22">
+      <c r="B22" t="s" s="0">
+        <v>155</v>
+      </c>
+      <c r="C22" t="s" s="0">
+        <v>156</v>
+      </c>
+    </row>
+    <row r="23">
+      <c r="B23" t="s" s="0">
+        <v>157</v>
+      </c>
+      <c r="C23" t="s" s="0">
+        <v>158</v>
+      </c>
+    </row>
+    <row r="24">
+      <c r="A24" t="s" s="12">
+        <v>159</v>
+      </c>
+      <c r="B24" t="s" s="0">
+        <v>160</v>
+      </c>
+      <c r="C24" t="s" s="0">
+        <v>161</v>
+      </c>
+    </row>
+    <row r="25">
+      <c r="B25" t="s" s="0">
+        <v>162</v>
+      </c>
+      <c r="C25" t="s" s="0">
+        <v>163</v>
+      </c>
+    </row>
+    <row r="26">
+      <c r="B26" t="s" s="0">
+        <v>164</v>
+      </c>
+      <c r="C26" t="s" s="0">
+        <v>165</v>
+      </c>
+    </row>
+    <row r="27">
+      <c r="B27" t="s" s="0">
+        <v>166</v>
+      </c>
+      <c r="C27" t="s" s="0">
+        <v>167</v>
+      </c>
+    </row>
+    <row r="28">
+      <c r="B28" t="s" s="0">
+        <v>168</v>
+      </c>
+      <c r="C28" t="s" s="0">
+        <v>169</v>
+      </c>
+    </row>
+    <row r="29">
+      <c r="B29" t="s" s="0">
+        <v>170</v>
+      </c>
+      <c r="C29" t="s" s="0">
+        <v>171</v>
+      </c>
+    </row>
+    <row r="30">
+      <c r="B30" t="s" s="0">
+        <v>172</v>
+      </c>
+      <c r="C30" t="s" s="0">
+        <v>173</v>
+      </c>
+    </row>
+    <row r="31">
+      <c r="B31" t="s" s="0">
+        <v>174</v>
+      </c>
+      <c r="C31" t="s" s="0">
+        <v>175</v>
+      </c>
+    </row>
+    <row r="32">
+      <c r="B32" t="s" s="0">
+        <v>176</v>
+      </c>
+      <c r="C32" t="s" s="0">
+        <v>177</v>
+      </c>
+    </row>
+    <row r="33">
+      <c r="B33" t="s" s="0">
+        <v>178</v>
+      </c>
+      <c r="C33" t="s" s="0">
+        <v>179</v>
+      </c>
+    </row>
+    <row r="34">
+      <c r="A34" t="s" s="13">
+        <v>180</v>
+      </c>
+      <c r="B34" t="s" s="0">
+        <v>181</v>
+      </c>
+      <c r="C34" t="s" s="0">
+        <v>182</v>
+      </c>
+    </row>
+    <row r="35">
+      <c r="B35" t="s" s="0">
+        <v>183</v>
+      </c>
+      <c r="C35" t="s" s="0">
+        <v>184</v>
+      </c>
+    </row>
+    <row r="36">
+      <c r="B36" t="s" s="0">
+        <v>185</v>
+      </c>
+      <c r="C36" t="s" s="0">
+        <v>186</v>
+      </c>
+    </row>
+    <row r="37">
+      <c r="B37" t="s" s="0">
+        <v>187</v>
+      </c>
+      <c r="C37" t="s" s="0">
+        <v>188</v>
+      </c>
+    </row>
+    <row r="38">
+      <c r="B38" t="s" s="0">
+        <v>189</v>
+      </c>
+      <c r="C38" t="s" s="0">
+        <v>190</v>
+      </c>
+    </row>
+    <row r="39">
+      <c r="B39" t="s" s="0">
+        <v>191</v>
+      </c>
+      <c r="C39" t="s" s="0">
+        <v>192</v>
+      </c>
+    </row>
+    <row r="40">
+      <c r="B40" t="s" s="0">
+        <v>193</v>
+      </c>
+      <c r="C40" t="s" s="0">
+        <v>194</v>
+      </c>
+    </row>
+    <row r="41">
+      <c r="B41" t="s" s="0">
+        <v>195</v>
+      </c>
+      <c r="C41" t="s" s="0">
+        <v>196</v>
+      </c>
+    </row>
+    <row r="42">
+      <c r="B42" t="s" s="0">
+        <v>7</v>
+      </c>
+      <c r="C42" t="s" s="0">
+        <v>197</v>
+      </c>
+    </row>
+    <row r="43">
+      <c r="B43" t="s" s="0">
+        <v>198</v>
+      </c>
+      <c r="C43" t="s" s="0">
+        <v>199</v>
+      </c>
+    </row>
+    <row r="44">
+      <c r="A44" t="s" s="14">
+        <v>200</v>
+      </c>
+      <c r="B44" t="s" s="0">
+        <v>201</v>
+      </c>
+      <c r="C44" t="s" s="0">
+        <v>202</v>
+      </c>
+    </row>
+    <row r="45">
+      <c r="B45" t="s" s="0">
+        <v>203</v>
+      </c>
+      <c r="C45" t="s" s="0">
+        <v>204</v>
+      </c>
+    </row>
+    <row r="46">
+      <c r="B46" t="s" s="0">
+        <v>205</v>
+      </c>
+      <c r="C46" t="s" s="0">
+        <v>206</v>
+      </c>
+    </row>
+    <row r="47">
+      <c r="B47" t="s" s="0">
+        <v>207</v>
+      </c>
+      <c r="C47" t="s" s="0">
+        <v>208</v>
+      </c>
+    </row>
+    <row r="48">
+      <c r="B48" t="s" s="0">
+        <v>209</v>
+      </c>
+      <c r="C48" t="s" s="0">
+        <v>210</v>
+      </c>
+    </row>
+    <row r="49">
+      <c r="B49" t="s" s="0">
+        <v>211</v>
+      </c>
+      <c r="C49" t="s" s="0">
+        <v>212</v>
+      </c>
+    </row>
+    <row r="50">
+      <c r="B50" t="s" s="0">
+        <v>213</v>
+      </c>
+      <c r="C50" t="s" s="0">
+        <v>214</v>
+      </c>
+    </row>
+    <row r="51">
+      <c r="B51" t="s" s="0">
+        <v>215</v>
+      </c>
+      <c r="C51" t="s" s="0">
+        <v>216</v>
+      </c>
+    </row>
+    <row r="52">
+      <c r="B52" t="s" s="0">
+        <v>217</v>
+      </c>
+      <c r="C52" t="s" s="0">
+        <v>218</v>
+      </c>
+    </row>
+    <row r="53">
+      <c r="B53" t="s" s="0">
+        <v>219</v>
+      </c>
+      <c r="C53" t="s" s="0">
+        <v>220</v>
+      </c>
+    </row>
+    <row r="54">
+      <c r="A54" t="s" s="15">
+        <v>221</v>
+      </c>
+      <c r="B54" t="s" s="0">
+        <v>222</v>
+      </c>
+      <c r="C54" t="s" s="0">
+        <v>223</v>
+      </c>
+    </row>
+    <row r="55">
+      <c r="B55" t="s" s="0">
+        <v>224</v>
+      </c>
+      <c r="C55" t="s" s="0">
+        <v>225</v>
+      </c>
+    </row>
+    <row r="56">
+      <c r="B56" t="s" s="0">
+        <v>226</v>
+      </c>
+      <c r="C56" t="s" s="0">
+        <v>227</v>
+      </c>
+    </row>
+    <row r="57">
+      <c r="B57" t="s" s="0">
+        <v>228</v>
+      </c>
+      <c r="C57" t="s" s="0">
+        <v>229</v>
+      </c>
+    </row>
+    <row r="58">
+      <c r="B58" t="s" s="0">
+        <v>230</v>
+      </c>
+      <c r="C58" t="s" s="0">
+        <v>231</v>
+      </c>
+    </row>
+    <row r="59">
+      <c r="B59" t="s" s="0">
+        <v>232</v>
+      </c>
+      <c r="C59" t="s" s="0">
+        <v>233</v>
+      </c>
+    </row>
+    <row r="60">
+      <c r="A60" t="s" s="16">
+        <v>234</v>
+      </c>
+      <c r="B60" t="s" s="0">
+        <v>235</v>
+      </c>
+      <c r="C60" t="s" s="0">
+        <v>236</v>
+      </c>
+    </row>
+    <row r="61">
+      <c r="B61" t="s" s="0">
+        <v>237</v>
+      </c>
+      <c r="C61" t="s" s="0">
+        <v>238</v>
+      </c>
+    </row>
+    <row r="62">
+      <c r="B62" t="s" s="0">
+        <v>239</v>
+      </c>
+      <c r="C62" t="s" s="0">
+        <v>240</v>
+      </c>
+    </row>
+    <row r="63">
+      <c r="B63" t="s" s="0">
+        <v>241</v>
+      </c>
+      <c r="C63" t="s" s="0">
+        <v>242</v>
+      </c>
+    </row>
+    <row r="64">
+      <c r="B64" t="s" s="0">
+        <v>243</v>
+      </c>
+      <c r="C64" t="s" s="0">
+        <v>244</v>
+      </c>
+    </row>
+    <row r="65">
+      <c r="B65" t="s" s="0">
+        <v>245</v>
+      </c>
+      <c r="C65" t="s" s="0">
+        <v>246</v>
+      </c>
+    </row>
+    <row r="66">
+      <c r="B66" t="s" s="0">
+        <v>247</v>
+      </c>
+      <c r="C66" t="s" s="0">
+        <v>248</v>
+      </c>
+    </row>
+    <row r="67">
+      <c r="B67" t="s" s="0">
+        <v>249</v>
+      </c>
+      <c r="C67" t="s" s="0">
+        <v>250</v>
+      </c>
+    </row>
+    <row r="68">
+      <c r="B68" t="s" s="0">
+        <v>251</v>
+      </c>
+      <c r="C68" t="s" s="0">
+        <v>252</v>
+      </c>
+    </row>
+    <row r="69">
+      <c r="B69" t="s" s="0">
+        <v>253</v>
+      </c>
+      <c r="C69" t="s" s="0">
+        <v>254</v>
+      </c>
+    </row>
+    <row r="70">
+      <c r="B70" t="s" s="0">
+        <v>255</v>
+      </c>
+      <c r="C70" t="s" s="0">
+        <v>256</v>
+      </c>
+    </row>
+    <row r="71">
+      <c r="B71" t="s" s="0">
+        <v>257</v>
+      </c>
+      <c r="C71" t="s" s="0">
+        <v>258</v>
+      </c>
+    </row>
+    <row r="72">
+      <c r="B72" t="s" s="0">
+        <v>259</v>
+      </c>
+      <c r="C72" t="s" s="0">
+        <v>260</v>
+      </c>
+    </row>
+    <row r="73">
+      <c r="B73" t="s" s="0">
+        <v>261</v>
+      </c>
+      <c r="C73" t="s" s="0">
+        <v>262</v>
+      </c>
+    </row>
+    <row r="74">
+      <c r="B74" t="s" s="0">
+        <v>263</v>
+      </c>
+      <c r="C74" t="s" s="0">
+        <v>264</v>
+      </c>
+    </row>
+    <row r="75">
+      <c r="B75" t="s" s="0">
+        <v>265</v>
+      </c>
+      <c r="C75" t="s" s="0">
+        <v>266</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
chore contant for excel-handling
</commit_message>
<xml_diff>
--- a/src/test/resources/CourseraAutomationData.xlsx
+++ b/src/test/resources/CourseraAutomationData.xlsx
@@ -45,7 +45,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="178" uniqueCount="100">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="445" uniqueCount="271">
   <si>
     <t>Search</t>
   </si>
@@ -345,6 +345,532 @@
   </si>
   <si>
     <t>2431</t>
+  </si>
+  <si>
+    <t>Full-Stack Web Development: PHP, HTML, CSS &amp; JavaScript</t>
+  </si>
+  <si>
+    <t>Rating Not Available</t>
+  </si>
+  <si>
+    <t>Must be valid email.
+example@yourdomain.com</t>
+  </si>
+  <si>
+    <t>Must be a phone number.
+503-555-1212</t>
+  </si>
+  <si>
+    <t>https://www.coursera.org/partners/huji</t>
+  </si>
+  <si>
+    <t>true</t>
+  </si>
+  <si>
+    <t>Hebrew University of Jerusalem</t>
+  </si>
+  <si>
+    <t>https://www.coursera.org/partners/technion</t>
+  </si>
+  <si>
+    <t>Technion - Israel Institute of Technology</t>
+  </si>
+  <si>
+    <t>https://www.coursera.org/partners/telaviv</t>
+  </si>
+  <si>
+    <t>Tel Aviv University</t>
+  </si>
+  <si>
+    <t>https://www.coursera.org/partners/yadvashem</t>
+  </si>
+  <si>
+    <t>Yad Vashem</t>
+  </si>
+  <si>
+    <t>O.P. Jindal Global University
+Bachelor of Science in Psychology
+World’s #1 university as per Times Higher Education Online Learning Rankings 2024
+Application due October 1, 2025</t>
+  </si>
+  <si>
+    <t>Georgetown University
+Bachelor of Arts in Liberal Studies
+Ranked #24 in the National University rankings (US News &amp; World Report, 2025)
+Application due October 15, 2025</t>
+  </si>
+  <si>
+    <t>University of North Texas
+Bachelor of Applied Arts and Sciences
+Ranked #25 for online Bachelor’s programs (U.S. News &amp; World Report, 2025)
+Application due July 31, 2025</t>
+  </si>
+  <si>
+    <t>Thanks for your interest in Coursera for Government
+We will get back to you soon!
+We look forward to sharing more information with you shortly. In the meantime, please explore a few examples of how Coursera for Government is preparing learners for jobs of the future.</t>
+  </si>
+  <si>
+    <t>More</t>
+  </si>
+  <si>
+    <t>Privacy</t>
+  </si>
+  <si>
+    <t>https://www.coursera.org/about/privacy</t>
+  </si>
+  <si>
+    <t>Manage Cookie Preferences</t>
+  </si>
+  <si>
+    <t>https://www.coursera.org/about/cookies-manage</t>
+  </si>
+  <si>
+    <t>Investors</t>
+  </si>
+  <si>
+    <t>https://investor.coursera.com/</t>
+  </si>
+  <si>
+    <t>Help</t>
+  </si>
+  <si>
+    <t>https://learner.coursera.help/hc</t>
+  </si>
+  <si>
+    <t>Accessibility</t>
+  </si>
+  <si>
+    <t>https://learner.coursera.help/hc/articles/360050668591-Accessibility-Statement</t>
+  </si>
+  <si>
+    <t>Articles</t>
+  </si>
+  <si>
+    <t>https://www.coursera.org/articles</t>
+  </si>
+  <si>
+    <t>Modern Slavery Statement</t>
+  </si>
+  <si>
+    <t>https://coursera_assets.s3.amazonaws.com/footer/Modern+Slavery+Statement+(approved+March+26%2C+2025).pdf</t>
+  </si>
+  <si>
+    <t>Affiliates</t>
+  </si>
+  <si>
+    <t>https://about.coursera.org/affiliates</t>
+  </si>
+  <si>
+    <t>Terms</t>
+  </si>
+  <si>
+    <t>https://www.coursera.org/about/terms</t>
+  </si>
+  <si>
+    <t>Press</t>
+  </si>
+  <si>
+    <t>https://www.coursera.org/about/press</t>
+  </si>
+  <si>
+    <t>Contact</t>
+  </si>
+  <si>
+    <t>https://www.coursera.org/about/contact</t>
+  </si>
+  <si>
+    <t>Directory</t>
+  </si>
+  <si>
+    <t>https://www.coursera.org/directory</t>
+  </si>
+  <si>
+    <t>Career Resources</t>
+  </si>
+  <si>
+    <t>How to Learn Artificial Intelligence</t>
+  </si>
+  <si>
+    <t>https://www.coursera.org/articles/how-to-learn-artificial-intelligence</t>
+  </si>
+  <si>
+    <t>Share your Coursera Learning Story</t>
+  </si>
+  <si>
+    <t>https://airtable.com/appxSsG2Dz9CjSpF8/pagCDDP2Uinw59CNP/form</t>
+  </si>
+  <si>
+    <t>Popular Cybersecurity Certifications</t>
+  </si>
+  <si>
+    <t>https://www.coursera.org/articles/popular-cybersecurity-certifications</t>
+  </si>
+  <si>
+    <t>How to Get a PMP Certification</t>
+  </si>
+  <si>
+    <t>https://www.coursera.org/articles/the-pmp-certification-a-guide-to-getting-started</t>
+  </si>
+  <si>
+    <t>Career Aptitude Test</t>
+  </si>
+  <si>
+    <t>https://www.coursera.org/resources/career-quiz</t>
+  </si>
+  <si>
+    <t>Career Development Resources</t>
+  </si>
+  <si>
+    <t>https://www.coursera.org/resources</t>
+  </si>
+  <si>
+    <t>Popular Data Analytics Certifications</t>
+  </si>
+  <si>
+    <t>https://www.coursera.org/articles/data-analytics-certification</t>
+  </si>
+  <si>
+    <t>Essential IT Certifications</t>
+  </si>
+  <si>
+    <t>https://www.coursera.org/articles/essential-it-certifications-entry-level-and-beginner</t>
+  </si>
+  <si>
+    <t>What Does a Data Analyst Do?</t>
+  </si>
+  <si>
+    <t>https://www.coursera.org/articles/what-does-a-data-analyst-do-a-career-guide</t>
+  </si>
+  <si>
+    <t>High-Income Skills to Learn</t>
+  </si>
+  <si>
+    <t>https://www.coursera.org/articles/high-income-skills</t>
+  </si>
+  <si>
+    <t>Analytical Skills</t>
+  </si>
+  <si>
+    <t>Data Science</t>
+  </si>
+  <si>
+    <t>https://www.coursera.org/courses?query=data%20science&amp;topic=Data%20Science</t>
+  </si>
+  <si>
+    <t>Artificial Intelligence</t>
+  </si>
+  <si>
+    <t>https://www.coursera.org/courses?query=artificial%20intelligence</t>
+  </si>
+  <si>
+    <t>Microsoft Power BI</t>
+  </si>
+  <si>
+    <t>https://www.coursera.org/courses?query=microsoft%20power%20bi</t>
+  </si>
+  <si>
+    <t>Big Data</t>
+  </si>
+  <si>
+    <t>https://www.coursera.org/courses?query=big%20data</t>
+  </si>
+  <si>
+    <t>Financial Modeling</t>
+  </si>
+  <si>
+    <t>https://www.coursera.org/courses?query=financial%20modeling</t>
+  </si>
+  <si>
+    <t>Data Analytics</t>
+  </si>
+  <si>
+    <t>https://www.coursera.org/courses?query=data%20analytics</t>
+  </si>
+  <si>
+    <t>Machine Learning</t>
+  </si>
+  <si>
+    <t>https://www.coursera.org/courses?query=machine%20learning&amp;skills=Machine%20Learning</t>
+  </si>
+  <si>
+    <t>Microsoft Excel</t>
+  </si>
+  <si>
+    <t>https://www.coursera.org/courses?query=microsoft%20excel</t>
+  </si>
+  <si>
+    <t>Business Analysis</t>
+  </si>
+  <si>
+    <t>https://www.coursera.org/courses?query=business%20analysis</t>
+  </si>
+  <si>
+    <t>SQL</t>
+  </si>
+  <si>
+    <t>https://www.coursera.org/courses?query=sql</t>
+  </si>
+  <si>
+    <t>Technical Skills</t>
+  </si>
+  <si>
+    <t>Ethical Hacking</t>
+  </si>
+  <si>
+    <t>https://www.coursera.org/courses?query=ethical%20hacking</t>
+  </si>
+  <si>
+    <t>DevOps</t>
+  </si>
+  <si>
+    <t>https://www.coursera.org/courses?query=devops</t>
+  </si>
+  <si>
+    <t>Generative AI</t>
+  </si>
+  <si>
+    <t>https://www.coursera.org/courses?query=generative%20ai</t>
+  </si>
+  <si>
+    <t>ChatGPT</t>
+  </si>
+  <si>
+    <t>https://www.coursera.org/courses?query=chatgpt</t>
+  </si>
+  <si>
+    <t>Coding</t>
+  </si>
+  <si>
+    <t>https://www.coursera.org/courses?query=coding</t>
+  </si>
+  <si>
+    <t>Computer Science</t>
+  </si>
+  <si>
+    <t>https://www.coursera.org/courses?query=computer%20science&amp;topic=Computer%20Science</t>
+  </si>
+  <si>
+    <t>Java Programming</t>
+  </si>
+  <si>
+    <t>https://www.coursera.org/courses?query=java</t>
+  </si>
+  <si>
+    <t>Cybersecurity</t>
+  </si>
+  <si>
+    <t>https://www.coursera.org/courses?query=cybersecurity</t>
+  </si>
+  <si>
+    <t>https://www.coursera.org/courses?query=web%20development</t>
+  </si>
+  <si>
+    <t>Python</t>
+  </si>
+  <si>
+    <t>https://www.coursera.org/courses?query=python</t>
+  </si>
+  <si>
+    <t>Business Skills</t>
+  </si>
+  <si>
+    <t>Google</t>
+  </si>
+  <si>
+    <t>https://www.coursera.org/courses?query=google</t>
+  </si>
+  <si>
+    <t>Project Management</t>
+  </si>
+  <si>
+    <t>https://www.coursera.org/courses?query=project%20management</t>
+  </si>
+  <si>
+    <t>Accounting</t>
+  </si>
+  <si>
+    <t>https://www.coursera.org/courses?query=accounting</t>
+  </si>
+  <si>
+    <t>IBM</t>
+  </si>
+  <si>
+    <t>https://www.coursera.org/courses?query=ibm</t>
+  </si>
+  <si>
+    <t>Finance</t>
+  </si>
+  <si>
+    <t>https://www.coursera.org/courses?query=finance&amp;skills=Finance</t>
+  </si>
+  <si>
+    <t>E-commerce</t>
+  </si>
+  <si>
+    <t>https://www.coursera.org/courses?query=e-commerce</t>
+  </si>
+  <si>
+    <t>Digital Marketing</t>
+  </si>
+  <si>
+    <t>https://www.coursera.org/courses?query=digital%20marketing</t>
+  </si>
+  <si>
+    <t>Social Media Marketing</t>
+  </si>
+  <si>
+    <t>https://www.coursera.org/courses?query=social%20media%20marketing</t>
+  </si>
+  <si>
+    <t>Graphic Design</t>
+  </si>
+  <si>
+    <t>https://www.coursera.org/courses?query=graphic%20design</t>
+  </si>
+  <si>
+    <t>Marketing</t>
+  </si>
+  <si>
+    <t>https://www.coursera.org/courses?query=marketing&amp;skills=Marketing</t>
+  </si>
+  <si>
+    <t>Community</t>
+  </si>
+  <si>
+    <t>Partners</t>
+  </si>
+  <si>
+    <t>https://www.coursera.org/partners</t>
+  </si>
+  <si>
+    <t>Tech Blog</t>
+  </si>
+  <si>
+    <t>https://medium.com/coursera-engineering</t>
+  </si>
+  <si>
+    <t>The Coursera Podcast</t>
+  </si>
+  <si>
+    <t>https://open.spotify.com/show/58M36bneU7REOofdPZxe6A</t>
+  </si>
+  <si>
+    <t>Beta Testers</t>
+  </si>
+  <si>
+    <t>https://www.coursera.support/s/article/360000152926-Become-a-Coursera-beta-tester</t>
+  </si>
+  <si>
+    <t>Learners</t>
+  </si>
+  <si>
+    <t>https://www.coursera.community/</t>
+  </si>
+  <si>
+    <t>Blog</t>
+  </si>
+  <si>
+    <t>https://blog.coursera.org/</t>
+  </si>
+  <si>
+    <t>Coursera</t>
+  </si>
+  <si>
+    <t>MasterTrack® Certificates</t>
+  </si>
+  <si>
+    <t>https://www.coursera.org/mastertrack</t>
+  </si>
+  <si>
+    <t>Leadership</t>
+  </si>
+  <si>
+    <t>https://about.coursera.org/leadership</t>
+  </si>
+  <si>
+    <t>Coursera Plus</t>
+  </si>
+  <si>
+    <t>https://www.coursera.org/courseraplus</t>
+  </si>
+  <si>
+    <t>Degrees</t>
+  </si>
+  <si>
+    <t>https://www.coursera.org/degrees</t>
+  </si>
+  <si>
+    <t>Become a Partner</t>
+  </si>
+  <si>
+    <t>https://partnerships.coursera.org/?utm_medium=coursera&amp;utm_source=partnerships&amp;utm_campaign=website&amp;utm_content=corp-to-home-footer-become-a-partner</t>
+  </si>
+  <si>
+    <t>For Enterprise</t>
+  </si>
+  <si>
+    <t>https://www.coursera.org/business?utm_campaign=website&amp;utm_content=corp-to-home-footer-for-enterprise&amp;utm_medium=coursera&amp;utm_source=enterprise</t>
+  </si>
+  <si>
+    <t>Careers</t>
+  </si>
+  <si>
+    <t>https://careers.coursera.com/</t>
+  </si>
+  <si>
+    <t>Professional Certificates</t>
+  </si>
+  <si>
+    <t>https://www.coursera.org/professional-certificate</t>
+  </si>
+  <si>
+    <t>What We Offer</t>
+  </si>
+  <si>
+    <t>https://about.coursera.org/how-coursera-works/</t>
+  </si>
+  <si>
+    <t>Catalog</t>
+  </si>
+  <si>
+    <t>https://www.coursera.org/browse</t>
+  </si>
+  <si>
+    <t>About</t>
+  </si>
+  <si>
+    <t>https://about.coursera.org/</t>
+  </si>
+  <si>
+    <t>For Government</t>
+  </si>
+  <si>
+    <t>https://www.coursera.org/government?utm_campaign=website&amp;utm_content=corp-to-home-footer-for-government&amp;utm_medium=coursera&amp;utm_source=enterprise</t>
+  </si>
+  <si>
+    <t>Social Impact</t>
+  </si>
+  <si>
+    <t>https://www.coursera.org/social-impact</t>
+  </si>
+  <si>
+    <t>ECTS Credit Recommendations</t>
+  </si>
+  <si>
+    <t>https://www.coursera.org/explore/ects-credit-recommendation</t>
+  </si>
+  <si>
+    <t>For Campus</t>
+  </si>
+  <si>
+    <t>https://www.coursera.org/campus?utm_campaign=website&amp;utm_content=corp-to-home-footer-for-campus&amp;utm_medium=coursera&amp;utm_source=enterprise</t>
+  </si>
+  <si>
+    <t>Free Courses</t>
+  </si>
+  <si>
+    <t>https://www.coursera.org/courses?query=free</t>
   </si>
 </sst>
 </file>
@@ -361,7 +887,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="5">
+  <fills count="7">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -384,6 +910,16 @@
       <patternFill patternType="solid">
         <fgColor theme="7" tint="0.39997558519241921"/>
         <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <fgColor indexed="17"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor indexed="17"/>
       </patternFill>
     </fill>
   </fills>
@@ -440,7 +976,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="10">
+  <cellXfs count="17">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
@@ -451,6 +987,13 @@
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFill="true"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -836,13 +1379,13 @@
         <v>5</v>
       </c>
       <c r="E2" s="1" t="s">
-        <v>33</v>
+        <v>100</v>
       </c>
       <c r="F2" s="1" t="s">
-        <v>34</v>
+        <v>101</v>
       </c>
       <c r="G2" s="1" t="s">
-        <v>35</v>
+        <v>39</v>
       </c>
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.35">
@@ -858,35 +1401,35 @@
     </row>
     <row r="4" spans="1:7" x14ac:dyDescent="0.35">
       <c r="E4" t="s" s="0">
-        <v>36</v>
+        <v>33</v>
       </c>
       <c r="F4" t="s" s="0">
-        <v>31</v>
+        <v>34</v>
       </c>
       <c r="G4" t="s" s="0">
-        <v>32</v>
+        <v>35</v>
       </c>
     </row>
     <row r="5" spans="1:7" x14ac:dyDescent="0.35">
       <c r="E5" t="s" s="0">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="F5" t="s" s="0">
-        <v>38</v>
+        <v>31</v>
       </c>
       <c r="G5" t="s" s="0">
-        <v>39</v>
+        <v>32</v>
       </c>
     </row>
     <row r="6" spans="1:7" x14ac:dyDescent="0.35">
       <c r="E6" t="s" s="0">
-        <v>40</v>
+        <v>37</v>
       </c>
       <c r="F6" t="s" s="0">
-        <v>31</v>
+        <v>38</v>
       </c>
       <c r="G6" t="s" s="0">
-        <v>32</v>
+        <v>39</v>
       </c>
     </row>
   </sheetData>
@@ -1219,8 +1762,12 @@
       <c r="A2" s="4" t="s">
         <v>13</v>
       </c>
-      <c r="B2" s="6"/>
-      <c r="C2" s="6"/>
+      <c r="B2" s="6" t="s">
+        <v>102</v>
+      </c>
+      <c r="C2" s="6" t="s">
+        <v>103</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -1229,7 +1776,7 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4877FAC2-2A6B-46DD-8D6C-E52B161D8FA6}">
-  <dimension ref="A1:C1"/>
+  <dimension ref="A1:C5"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="D11" sqref="D11"/>
@@ -1253,6 +1800,50 @@
         <v>16</v>
       </c>
     </row>
+    <row r="2">
+      <c r="A2" t="s" s="0">
+        <v>104</v>
+      </c>
+      <c r="B2" t="s" s="0">
+        <v>105</v>
+      </c>
+      <c r="C2" t="s" s="0">
+        <v>106</v>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" t="s" s="0">
+        <v>107</v>
+      </c>
+      <c r="B3" t="s" s="0">
+        <v>105</v>
+      </c>
+      <c r="C3" t="s" s="0">
+        <v>108</v>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" t="s" s="0">
+        <v>109</v>
+      </c>
+      <c r="B4" t="s" s="0">
+        <v>105</v>
+      </c>
+      <c r="C4" t="s" s="0">
+        <v>110</v>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" t="s" s="0">
+        <v>111</v>
+      </c>
+      <c r="B5" t="s" s="0">
+        <v>105</v>
+      </c>
+      <c r="C5" t="s" s="0">
+        <v>112</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -1260,7 +1851,7 @@
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{50AE5632-D04D-4B85-93F9-0760C2D5CD44}">
-  <dimension ref="A1"/>
+  <dimension ref="A1:A4"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -1272,6 +1863,21 @@
     <row r="1" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A1" s="3" t="s">
         <v>17</v>
+      </c>
+    </row>
+    <row r="2">
+      <c r="A2" t="s" s="0">
+        <v>113</v>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" t="s" s="0">
+        <v>114</v>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" t="s" s="0">
+        <v>115</v>
       </c>
     </row>
   </sheetData>
@@ -1395,6 +2001,9 @@
       <c r="A2" s="4" t="s">
         <v>13</v>
       </c>
+      <c r="B2" t="s" s="0">
+        <v>116</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -1403,7 +2012,7 @@
 
 <file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8A3EB322-FF18-442E-8BCD-C9A28A47FC30}">
-  <dimension ref="A1:C1"/>
+  <dimension ref="A1:C75"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="B3" sqref="B3"/>
@@ -1422,6 +2031,619 @@
         <v>29</v>
       </c>
     </row>
+    <row r="2">
+      <c r="A2" t="s" s="10">
+        <v>117</v>
+      </c>
+      <c r="B2" t="s" s="0">
+        <v>118</v>
+      </c>
+      <c r="C2" t="s" s="0">
+        <v>119</v>
+      </c>
+    </row>
+    <row r="3">
+      <c r="B3" t="s" s="0">
+        <v>120</v>
+      </c>
+      <c r="C3" t="s" s="0">
+        <v>121</v>
+      </c>
+    </row>
+    <row r="4">
+      <c r="B4" t="s" s="0">
+        <v>122</v>
+      </c>
+      <c r="C4" t="s" s="0">
+        <v>123</v>
+      </c>
+    </row>
+    <row r="5">
+      <c r="B5" t="s" s="0">
+        <v>124</v>
+      </c>
+      <c r="C5" t="s" s="0">
+        <v>125</v>
+      </c>
+    </row>
+    <row r="6">
+      <c r="B6" t="s" s="0">
+        <v>126</v>
+      </c>
+      <c r="C6" t="s" s="0">
+        <v>127</v>
+      </c>
+    </row>
+    <row r="7">
+      <c r="B7" t="s" s="0">
+        <v>128</v>
+      </c>
+      <c r="C7" t="s" s="0">
+        <v>129</v>
+      </c>
+    </row>
+    <row r="8">
+      <c r="B8" t="s" s="0">
+        <v>130</v>
+      </c>
+      <c r="C8" t="s" s="0">
+        <v>131</v>
+      </c>
+    </row>
+    <row r="9">
+      <c r="B9" t="s" s="0">
+        <v>132</v>
+      </c>
+      <c r="C9" t="s" s="0">
+        <v>133</v>
+      </c>
+    </row>
+    <row r="10">
+      <c r="B10" t="s" s="0">
+        <v>134</v>
+      </c>
+      <c r="C10" t="s" s="0">
+        <v>135</v>
+      </c>
+    </row>
+    <row r="11">
+      <c r="B11" t="s" s="0">
+        <v>136</v>
+      </c>
+      <c r="C11" t="s" s="0">
+        <v>137</v>
+      </c>
+    </row>
+    <row r="12">
+      <c r="B12" t="s" s="0">
+        <v>138</v>
+      </c>
+      <c r="C12" t="s" s="0">
+        <v>139</v>
+      </c>
+    </row>
+    <row r="13">
+      <c r="B13" t="s" s="0">
+        <v>140</v>
+      </c>
+      <c r="C13" t="s" s="0">
+        <v>141</v>
+      </c>
+    </row>
+    <row r="14">
+      <c r="A14" t="s" s="11">
+        <v>142</v>
+      </c>
+      <c r="B14" t="s" s="0">
+        <v>143</v>
+      </c>
+      <c r="C14" t="s" s="0">
+        <v>144</v>
+      </c>
+    </row>
+    <row r="15">
+      <c r="B15" t="s" s="0">
+        <v>145</v>
+      </c>
+      <c r="C15" t="s" s="0">
+        <v>146</v>
+      </c>
+    </row>
+    <row r="16">
+      <c r="B16" t="s" s="0">
+        <v>147</v>
+      </c>
+      <c r="C16" t="s" s="0">
+        <v>148</v>
+      </c>
+    </row>
+    <row r="17">
+      <c r="B17" t="s" s="0">
+        <v>149</v>
+      </c>
+      <c r="C17" t="s" s="0">
+        <v>150</v>
+      </c>
+    </row>
+    <row r="18">
+      <c r="B18" t="s" s="0">
+        <v>151</v>
+      </c>
+      <c r="C18" t="s" s="0">
+        <v>152</v>
+      </c>
+    </row>
+    <row r="19">
+      <c r="B19" t="s" s="0">
+        <v>153</v>
+      </c>
+      <c r="C19" t="s" s="0">
+        <v>154</v>
+      </c>
+    </row>
+    <row r="20">
+      <c r="B20" t="s" s="0">
+        <v>155</v>
+      </c>
+      <c r="C20" t="s" s="0">
+        <v>156</v>
+      </c>
+    </row>
+    <row r="21">
+      <c r="B21" t="s" s="0">
+        <v>157</v>
+      </c>
+      <c r="C21" t="s" s="0">
+        <v>158</v>
+      </c>
+    </row>
+    <row r="22">
+      <c r="B22" t="s" s="0">
+        <v>159</v>
+      </c>
+      <c r="C22" t="s" s="0">
+        <v>160</v>
+      </c>
+    </row>
+    <row r="23">
+      <c r="B23" t="s" s="0">
+        <v>161</v>
+      </c>
+      <c r="C23" t="s" s="0">
+        <v>162</v>
+      </c>
+    </row>
+    <row r="24">
+      <c r="A24" t="s" s="12">
+        <v>163</v>
+      </c>
+      <c r="B24" t="s" s="0">
+        <v>164</v>
+      </c>
+      <c r="C24" t="s" s="0">
+        <v>165</v>
+      </c>
+    </row>
+    <row r="25">
+      <c r="B25" t="s" s="0">
+        <v>166</v>
+      </c>
+      <c r="C25" t="s" s="0">
+        <v>167</v>
+      </c>
+    </row>
+    <row r="26">
+      <c r="B26" t="s" s="0">
+        <v>168</v>
+      </c>
+      <c r="C26" t="s" s="0">
+        <v>169</v>
+      </c>
+    </row>
+    <row r="27">
+      <c r="B27" t="s" s="0">
+        <v>170</v>
+      </c>
+      <c r="C27" t="s" s="0">
+        <v>171</v>
+      </c>
+    </row>
+    <row r="28">
+      <c r="B28" t="s" s="0">
+        <v>172</v>
+      </c>
+      <c r="C28" t="s" s="0">
+        <v>173</v>
+      </c>
+    </row>
+    <row r="29">
+      <c r="B29" t="s" s="0">
+        <v>174</v>
+      </c>
+      <c r="C29" t="s" s="0">
+        <v>175</v>
+      </c>
+    </row>
+    <row r="30">
+      <c r="B30" t="s" s="0">
+        <v>176</v>
+      </c>
+      <c r="C30" t="s" s="0">
+        <v>177</v>
+      </c>
+    </row>
+    <row r="31">
+      <c r="B31" t="s" s="0">
+        <v>178</v>
+      </c>
+      <c r="C31" t="s" s="0">
+        <v>179</v>
+      </c>
+    </row>
+    <row r="32">
+      <c r="B32" t="s" s="0">
+        <v>180</v>
+      </c>
+      <c r="C32" t="s" s="0">
+        <v>181</v>
+      </c>
+    </row>
+    <row r="33">
+      <c r="B33" t="s" s="0">
+        <v>182</v>
+      </c>
+      <c r="C33" t="s" s="0">
+        <v>183</v>
+      </c>
+    </row>
+    <row r="34">
+      <c r="A34" t="s" s="13">
+        <v>184</v>
+      </c>
+      <c r="B34" t="s" s="0">
+        <v>185</v>
+      </c>
+      <c r="C34" t="s" s="0">
+        <v>186</v>
+      </c>
+    </row>
+    <row r="35">
+      <c r="B35" t="s" s="0">
+        <v>187</v>
+      </c>
+      <c r="C35" t="s" s="0">
+        <v>188</v>
+      </c>
+    </row>
+    <row r="36">
+      <c r="B36" t="s" s="0">
+        <v>189</v>
+      </c>
+      <c r="C36" t="s" s="0">
+        <v>190</v>
+      </c>
+    </row>
+    <row r="37">
+      <c r="B37" t="s" s="0">
+        <v>191</v>
+      </c>
+      <c r="C37" t="s" s="0">
+        <v>192</v>
+      </c>
+    </row>
+    <row r="38">
+      <c r="B38" t="s" s="0">
+        <v>193</v>
+      </c>
+      <c r="C38" t="s" s="0">
+        <v>194</v>
+      </c>
+    </row>
+    <row r="39">
+      <c r="B39" t="s" s="0">
+        <v>195</v>
+      </c>
+      <c r="C39" t="s" s="0">
+        <v>196</v>
+      </c>
+    </row>
+    <row r="40">
+      <c r="B40" t="s" s="0">
+        <v>197</v>
+      </c>
+      <c r="C40" t="s" s="0">
+        <v>198</v>
+      </c>
+    </row>
+    <row r="41">
+      <c r="B41" t="s" s="0">
+        <v>199</v>
+      </c>
+      <c r="C41" t="s" s="0">
+        <v>200</v>
+      </c>
+    </row>
+    <row r="42">
+      <c r="B42" t="s" s="0">
+        <v>7</v>
+      </c>
+      <c r="C42" t="s" s="0">
+        <v>201</v>
+      </c>
+    </row>
+    <row r="43">
+      <c r="B43" t="s" s="0">
+        <v>202</v>
+      </c>
+      <c r="C43" t="s" s="0">
+        <v>203</v>
+      </c>
+    </row>
+    <row r="44">
+      <c r="A44" t="s" s="14">
+        <v>204</v>
+      </c>
+      <c r="B44" t="s" s="0">
+        <v>205</v>
+      </c>
+      <c r="C44" t="s" s="0">
+        <v>206</v>
+      </c>
+    </row>
+    <row r="45">
+      <c r="B45" t="s" s="0">
+        <v>207</v>
+      </c>
+      <c r="C45" t="s" s="0">
+        <v>208</v>
+      </c>
+    </row>
+    <row r="46">
+      <c r="B46" t="s" s="0">
+        <v>209</v>
+      </c>
+      <c r="C46" t="s" s="0">
+        <v>210</v>
+      </c>
+    </row>
+    <row r="47">
+      <c r="B47" t="s" s="0">
+        <v>211</v>
+      </c>
+      <c r="C47" t="s" s="0">
+        <v>212</v>
+      </c>
+    </row>
+    <row r="48">
+      <c r="B48" t="s" s="0">
+        <v>213</v>
+      </c>
+      <c r="C48" t="s" s="0">
+        <v>214</v>
+      </c>
+    </row>
+    <row r="49">
+      <c r="B49" t="s" s="0">
+        <v>215</v>
+      </c>
+      <c r="C49" t="s" s="0">
+        <v>216</v>
+      </c>
+    </row>
+    <row r="50">
+      <c r="B50" t="s" s="0">
+        <v>217</v>
+      </c>
+      <c r="C50" t="s" s="0">
+        <v>218</v>
+      </c>
+    </row>
+    <row r="51">
+      <c r="B51" t="s" s="0">
+        <v>219</v>
+      </c>
+      <c r="C51" t="s" s="0">
+        <v>220</v>
+      </c>
+    </row>
+    <row r="52">
+      <c r="B52" t="s" s="0">
+        <v>221</v>
+      </c>
+      <c r="C52" t="s" s="0">
+        <v>222</v>
+      </c>
+    </row>
+    <row r="53">
+      <c r="B53" t="s" s="0">
+        <v>223</v>
+      </c>
+      <c r="C53" t="s" s="0">
+        <v>224</v>
+      </c>
+    </row>
+    <row r="54">
+      <c r="A54" t="s" s="15">
+        <v>225</v>
+      </c>
+      <c r="B54" t="s" s="0">
+        <v>226</v>
+      </c>
+      <c r="C54" t="s" s="0">
+        <v>227</v>
+      </c>
+    </row>
+    <row r="55">
+      <c r="B55" t="s" s="0">
+        <v>228</v>
+      </c>
+      <c r="C55" t="s" s="0">
+        <v>229</v>
+      </c>
+    </row>
+    <row r="56">
+      <c r="B56" t="s" s="0">
+        <v>230</v>
+      </c>
+      <c r="C56" t="s" s="0">
+        <v>231</v>
+      </c>
+    </row>
+    <row r="57">
+      <c r="B57" t="s" s="0">
+        <v>232</v>
+      </c>
+      <c r="C57" t="s" s="0">
+        <v>233</v>
+      </c>
+    </row>
+    <row r="58">
+      <c r="B58" t="s" s="0">
+        <v>234</v>
+      </c>
+      <c r="C58" t="s" s="0">
+        <v>235</v>
+      </c>
+    </row>
+    <row r="59">
+      <c r="B59" t="s" s="0">
+        <v>236</v>
+      </c>
+      <c r="C59" t="s" s="0">
+        <v>237</v>
+      </c>
+    </row>
+    <row r="60">
+      <c r="A60" t="s" s="16">
+        <v>238</v>
+      </c>
+      <c r="B60" t="s" s="0">
+        <v>239</v>
+      </c>
+      <c r="C60" t="s" s="0">
+        <v>240</v>
+      </c>
+    </row>
+    <row r="61">
+      <c r="B61" t="s" s="0">
+        <v>241</v>
+      </c>
+      <c r="C61" t="s" s="0">
+        <v>242</v>
+      </c>
+    </row>
+    <row r="62">
+      <c r="B62" t="s" s="0">
+        <v>243</v>
+      </c>
+      <c r="C62" t="s" s="0">
+        <v>244</v>
+      </c>
+    </row>
+    <row r="63">
+      <c r="B63" t="s" s="0">
+        <v>245</v>
+      </c>
+      <c r="C63" t="s" s="0">
+        <v>246</v>
+      </c>
+    </row>
+    <row r="64">
+      <c r="B64" t="s" s="0">
+        <v>247</v>
+      </c>
+      <c r="C64" t="s" s="0">
+        <v>248</v>
+      </c>
+    </row>
+    <row r="65">
+      <c r="B65" t="s" s="0">
+        <v>249</v>
+      </c>
+      <c r="C65" t="s" s="0">
+        <v>250</v>
+      </c>
+    </row>
+    <row r="66">
+      <c r="B66" t="s" s="0">
+        <v>251</v>
+      </c>
+      <c r="C66" t="s" s="0">
+        <v>252</v>
+      </c>
+    </row>
+    <row r="67">
+      <c r="B67" t="s" s="0">
+        <v>253</v>
+      </c>
+      <c r="C67" t="s" s="0">
+        <v>254</v>
+      </c>
+    </row>
+    <row r="68">
+      <c r="B68" t="s" s="0">
+        <v>255</v>
+      </c>
+      <c r="C68" t="s" s="0">
+        <v>256</v>
+      </c>
+    </row>
+    <row r="69">
+      <c r="B69" t="s" s="0">
+        <v>257</v>
+      </c>
+      <c r="C69" t="s" s="0">
+        <v>258</v>
+      </c>
+    </row>
+    <row r="70">
+      <c r="B70" t="s" s="0">
+        <v>259</v>
+      </c>
+      <c r="C70" t="s" s="0">
+        <v>260</v>
+      </c>
+    </row>
+    <row r="71">
+      <c r="B71" t="s" s="0">
+        <v>261</v>
+      </c>
+      <c r="C71" t="s" s="0">
+        <v>262</v>
+      </c>
+    </row>
+    <row r="72">
+      <c r="B72" t="s" s="0">
+        <v>263</v>
+      </c>
+      <c r="C72" t="s" s="0">
+        <v>264</v>
+      </c>
+    </row>
+    <row r="73">
+      <c r="B73" t="s" s="0">
+        <v>265</v>
+      </c>
+      <c r="C73" t="s" s="0">
+        <v>266</v>
+      </c>
+    </row>
+    <row r="74">
+      <c r="B74" t="s" s="0">
+        <v>267</v>
+      </c>
+      <c r="C74" t="s" s="0">
+        <v>268</v>
+      </c>
+    </row>
+    <row r="75">
+      <c r="B75" t="s" s="0">
+        <v>269</v>
+      </c>
+      <c r="C75" t="s" s="0">
+        <v>270</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>